<commit_message>
Correcciones reunion unai (documentacion)
</commit_message>
<xml_diff>
--- a/001-Planificacion Diagrama de gant ( plantilla wpsoficce).xlsx
+++ b/001-Planificacion Diagrama de gant ( plantilla wpsoficce).xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="15780" windowHeight="8592"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ProjectSchedule!$1:$42</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">ProjectSchedule!$4:$6</definedName>
     <definedName name="task_end" localSheetId="0">ProjectSchedule!$D1</definedName>
     <definedName name="task_progress" localSheetId="0">ProjectSchedule!#REF!</definedName>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>TRABAJO ALTERNATIVO PBL</t>
   </si>
@@ -93,19 +93,25 @@
     <t>Ejercicio de proyecto completo</t>
   </si>
   <si>
-    <t>Correcciones y ajustes del trabajo</t>
+    <t>Ajustes y correcciones</t>
   </si>
   <si>
-    <t>Milestone 1</t>
+    <t>Apartado basico ( entrada, stub-skeleton, naming server, serializacion)</t>
   </si>
   <si>
     <t>Hacer apartado entrada - Documentacion</t>
   </si>
   <si>
-    <t>Apartado basico - platear ejercicios</t>
+    <t>Apartado basico - ejercicios (plantear, codificar)</t>
   </si>
   <si>
-    <t>Apartado basico - codificar ejercicis</t>
+    <t>Ejercicio de stub-skeleton 2</t>
+  </si>
+  <si>
+    <t>Ejercicios de naming server 3-4</t>
+  </si>
+  <si>
+    <t>Ejercicios de serializacion 3</t>
   </si>
   <si>
     <t>Apartado basico - Documentacion</t>
@@ -114,40 +120,43 @@
     <t>Reunion segimiento</t>
   </si>
   <si>
-    <t>Ajustes y correcciones</t>
+    <t xml:space="preserve">Apartado de seguridad </t>
   </si>
   <si>
-    <t>Milestone 2</t>
+    <t>Apartado de seguridad- ejercicios (plantear, codificar)</t>
   </si>
   <si>
-    <t>Apartado de seguridad- plantear ejercios</t>
+    <t>Ejercicios de buscar Vulnerabilidades  2</t>
   </si>
   <si>
-    <t>Apartado de seguridad- codificar ejercicios</t>
+    <t>Ejercicios  de securizar la aplicacion 1-2 (con RMISecurity manager)</t>
   </si>
   <si>
     <t>Apartado de seguridad- Documentacion</t>
   </si>
   <si>
-    <t>Milestone 3</t>
+    <t>Apartado de carga dinamica</t>
   </si>
   <si>
-    <t>Carga dinamica- plantear ejercios</t>
+    <t>Apartado Carga dinamica-ejercicios (plantear ,codificar)</t>
   </si>
   <si>
-    <t>Carga dinamica- codificar ejercios</t>
+    <t>?</t>
   </si>
   <si>
     <t>Carga dinamica- documentacion</t>
   </si>
   <si>
-    <t>Milestone 4</t>
+    <t xml:space="preserve">Ejercicios complejos </t>
   </si>
   <si>
-    <t>Ejercicio completo -Planteamiento</t>
+    <t>Ejercicio completo-ejercicios (plantear, codificar)</t>
   </si>
   <si>
-    <t>Ejercicio completo - codificacion</t>
+    <t>Ejercicio Objetos remotos y seguridad ( repartidores)</t>
+  </si>
+  <si>
+    <t>Ejercicio carga dinamica ( procesador calculos /finanzas?)</t>
   </si>
   <si>
     <t>Ejercicio completo - documentacion</t>
@@ -161,14 +170,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="180" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="182" formatCode="d"/>
-    <numFmt numFmtId="183" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="182" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="183" formatCode="d"/>
   </numFmts>
   <fonts count="38">
     <font>
@@ -280,10 +289,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -295,39 +305,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -357,14 +335,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -373,7 +343,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,15 +373,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -417,7 +404,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,7 +443,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,6 +489,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7FAFC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,7 +548,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF44678E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A6F9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,31 +608,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -587,6 +632,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -599,61 +680,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,36 +823,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -850,13 +847,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -866,6 +867,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -893,21 +909,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -915,132 +942,132 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1052,10 +1079,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1077,10 +1104,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1098,10 +1125,10 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1113,106 +1140,115 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="182" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="9" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="11" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="11" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="9" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="9" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1224,25 +1260,28 @@
     <xf numFmtId="181" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="181" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1251,7 +1290,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1260,10 +1302,10 @@
     <xf numFmtId="181" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="15" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="15" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1522,16 +1564,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
-      <color rgb="00215881"/>
-      <color rgb="0042648A"/>
-      <color rgb="00969696"/>
-      <color rgb="00C0C0C0"/>
-      <color rgb="00427FC2"/>
+      <color rgb="00B8CCE4"/>
+      <color rgb="004A6F9C"/>
+      <color rgb="00F9EEEE"/>
+      <color rgb="00F2DCDB"/>
+      <color rgb="00F8EBEB"/>
+      <color rgb="00F9FBF4"/>
+      <color rgb="00FFFFFF"/>
       <color rgb="0044678E"/>
-      <color rgb="004A6F9C"/>
-      <color rgb="003969AD"/>
-      <color rgb="00000000"/>
-      <color rgb="00B8CCE4"/>
+      <color rgb="00E8EEF4"/>
+      <color rgb="00F7FAFC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1802,20 +1844,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BJ55"/>
+  <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="2.71296296296296" customWidth="1"/>
-    <col min="2" max="2" width="45.5648148148148" customWidth="1"/>
+    <col min="2" max="2" width="61.8148148148148" customWidth="1"/>
     <col min="3" max="3" width="10.4259259259259" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.4259259259259" customWidth="1"/>
+    <col min="4" max="4" width="11.3148148148148" customWidth="1"/>
     <col min="5" max="5" width="2.71296296296296" customWidth="1"/>
     <col min="6" max="6" width="6.13888888888889" hidden="1" customWidth="1"/>
     <col min="7" max="62" width="2.57407407407407" customWidth="1"/>
@@ -2023,7 +2065,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="64"/>
+      <c r="M4" s="67"/>
       <c r="N4" s="9">
         <f>N5</f>
         <v>45040</v>
@@ -2033,7 +2075,7 @@
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
-      <c r="T4" s="64"/>
+      <c r="T4" s="67"/>
       <c r="U4" s="9">
         <f>U5</f>
         <v>45047</v>
@@ -2043,7 +2085,7 @@
       <c r="X4" s="10"/>
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
-      <c r="AA4" s="64"/>
+      <c r="AA4" s="67"/>
       <c r="AB4" s="9">
         <f>AB5</f>
         <v>45054</v>
@@ -2053,7 +2095,7 @@
       <c r="AE4" s="10"/>
       <c r="AF4" s="10"/>
       <c r="AG4" s="10"/>
-      <c r="AH4" s="64"/>
+      <c r="AH4" s="67"/>
       <c r="AI4" s="9">
         <f>AI5</f>
         <v>45061</v>
@@ -2063,7 +2105,7 @@
       <c r="AL4" s="10"/>
       <c r="AM4" s="10"/>
       <c r="AN4" s="10"/>
-      <c r="AO4" s="64"/>
+      <c r="AO4" s="67"/>
       <c r="AP4" s="9">
         <f>AP5</f>
         <v>45068</v>
@@ -2073,7 +2115,7 @@
       <c r="AS4" s="10"/>
       <c r="AT4" s="10"/>
       <c r="AU4" s="10"/>
-      <c r="AV4" s="64"/>
+      <c r="AV4" s="67"/>
       <c r="AW4" s="9">
         <f>AW5</f>
         <v>45075</v>
@@ -2083,17 +2125,17 @@
       <c r="AZ4" s="10"/>
       <c r="BA4" s="10"/>
       <c r="BB4" s="10"/>
-      <c r="BC4" s="64"/>
-      <c r="BD4" s="70">
+      <c r="BC4" s="67"/>
+      <c r="BD4" s="74">
         <f>BD5</f>
         <v>45082</v>
       </c>
-      <c r="BE4" s="75"/>
-      <c r="BF4" s="75"/>
-      <c r="BG4" s="75"/>
-      <c r="BH4" s="75"/>
-      <c r="BI4" s="75"/>
-      <c r="BJ4" s="76"/>
+      <c r="BE4" s="80"/>
+      <c r="BF4" s="80"/>
+      <c r="BG4" s="80"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="80"/>
+      <c r="BJ4" s="81"/>
     </row>
     <row r="5" spans="1:62">
       <c r="A5" s="11"/>
@@ -2126,7 +2168,7 @@
         <f t="shared" si="0"/>
         <v>45038</v>
       </c>
-      <c r="M5" s="65">
+      <c r="M5" s="68">
         <f t="shared" si="0"/>
         <v>45039</v>
       </c>
@@ -2154,7 +2196,7 @@
         <f t="shared" si="0"/>
         <v>45045</v>
       </c>
-      <c r="T5" s="65">
+      <c r="T5" s="68">
         <f t="shared" si="0"/>
         <v>45046</v>
       </c>
@@ -2182,7 +2224,7 @@
         <f t="shared" si="0"/>
         <v>45052</v>
       </c>
-      <c r="AA5" s="65">
+      <c r="AA5" s="68">
         <f t="shared" si="0"/>
         <v>45053</v>
       </c>
@@ -2210,7 +2252,7 @@
         <f t="shared" si="0"/>
         <v>45059</v>
       </c>
-      <c r="AH5" s="65">
+      <c r="AH5" s="68">
         <f t="shared" si="0"/>
         <v>45060</v>
       </c>
@@ -2238,7 +2280,7 @@
         <f t="shared" si="0"/>
         <v>45066</v>
       </c>
-      <c r="AO5" s="65">
+      <c r="AO5" s="68">
         <f t="shared" si="0"/>
         <v>45067</v>
       </c>
@@ -2266,7 +2308,7 @@
         <f t="shared" si="0"/>
         <v>45073</v>
       </c>
-      <c r="AV5" s="65">
+      <c r="AV5" s="68">
         <f t="shared" si="0"/>
         <v>45074</v>
       </c>
@@ -2294,35 +2336,35 @@
         <f t="shared" si="1"/>
         <v>45080</v>
       </c>
-      <c r="BC5" s="65">
+      <c r="BC5" s="68">
         <f t="shared" si="1"/>
         <v>45081</v>
       </c>
-      <c r="BD5" s="71">
+      <c r="BD5" s="75">
         <f t="shared" si="1"/>
         <v>45082</v>
       </c>
-      <c r="BE5" s="77">
+      <c r="BE5" s="82">
         <f t="shared" si="1"/>
         <v>45083</v>
       </c>
-      <c r="BF5" s="77">
+      <c r="BF5" s="82">
         <f t="shared" ref="BF5:BJ5" si="2">BE5+1</f>
         <v>45084</v>
       </c>
-      <c r="BG5" s="77">
+      <c r="BG5" s="82">
         <f t="shared" si="2"/>
         <v>45085</v>
       </c>
-      <c r="BH5" s="77">
+      <c r="BH5" s="82">
         <f t="shared" si="2"/>
         <v>45086</v>
       </c>
-      <c r="BI5" s="77">
+      <c r="BI5" s="82">
         <f t="shared" si="2"/>
         <v>45087</v>
       </c>
-      <c r="BJ5" s="78">
+      <c r="BJ5" s="83">
         <f t="shared" si="2"/>
         <v>45088</v>
       </c>
@@ -2538,31 +2580,31 @@
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="BD6" s="72" t="str">
+      <c r="BD6" s="76" t="str">
         <f t="shared" si="4"/>
         <v>M</v>
       </c>
-      <c r="BE6" s="72" t="str">
+      <c r="BE6" s="76" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="BF6" s="72" t="str">
+      <c r="BF6" s="76" t="str">
         <f t="shared" si="4"/>
         <v>W</v>
       </c>
-      <c r="BG6" s="72" t="str">
+      <c r="BG6" s="76" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="BH6" s="72" t="str">
+      <c r="BH6" s="76" t="str">
         <f t="shared" si="4"/>
         <v>F</v>
       </c>
-      <c r="BI6" s="72" t="str">
+      <c r="BI6" s="76" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="BJ6" s="72" t="str">
+      <c r="BJ6" s="76" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
@@ -2628,15 +2670,15 @@
       <c r="BA7" s="24"/>
       <c r="BB7" s="24"/>
       <c r="BC7" s="24"/>
-      <c r="BD7" s="73"/>
-      <c r="BE7" s="73"/>
-      <c r="BF7" s="73"/>
-      <c r="BG7" s="73"/>
-      <c r="BH7" s="73"/>
-      <c r="BI7" s="73"/>
-      <c r="BJ7" s="73"/>
+      <c r="BD7" s="77"/>
+      <c r="BE7" s="77"/>
+      <c r="BF7" s="77"/>
+      <c r="BG7" s="77"/>
+      <c r="BH7" s="77"/>
+      <c r="BI7" s="77"/>
+      <c r="BJ7" s="77"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="21" spans="1:62">
+    <row r="8" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A8" s="16"/>
       <c r="B8" s="25" t="s">
         <v>7</v>
@@ -2654,9 +2696,9 @@
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="67"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="24"/>
       <c r="M8" s="24"/>
       <c r="N8" s="24"/>
@@ -2701,15 +2743,15 @@
       <c r="BA8" s="24"/>
       <c r="BB8" s="24"/>
       <c r="BC8" s="24"/>
-      <c r="BD8" s="73"/>
-      <c r="BE8" s="73"/>
-      <c r="BF8" s="73"/>
-      <c r="BG8" s="73"/>
-      <c r="BH8" s="73"/>
-      <c r="BI8" s="73"/>
-      <c r="BJ8" s="73"/>
+      <c r="BD8" s="77"/>
+      <c r="BE8" s="77"/>
+      <c r="BF8" s="77"/>
+      <c r="BG8" s="77"/>
+      <c r="BH8" s="77"/>
+      <c r="BI8" s="77"/>
+      <c r="BJ8" s="77"/>
     </row>
-    <row r="9" s="1" customFormat="1" ht="21" spans="1:62">
+    <row r="9" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A9" s="16"/>
       <c r="B9" s="25" t="s">
         <v>8</v>
@@ -2727,9 +2769,9 @@
       </c>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="67"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
       <c r="L9" s="24"/>
       <c r="M9" s="24"/>
       <c r="N9" s="24"/>
@@ -2737,8 +2779,8 @@
       <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
-      <c r="S9" s="69"/>
-      <c r="T9" s="69"/>
+      <c r="S9" s="72"/>
+      <c r="T9" s="72"/>
       <c r="U9" s="24"/>
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
@@ -2774,13 +2816,13 @@
       <c r="BA9" s="24"/>
       <c r="BB9" s="24"/>
       <c r="BC9" s="24"/>
-      <c r="BD9" s="73"/>
-      <c r="BE9" s="73"/>
-      <c r="BF9" s="73"/>
-      <c r="BG9" s="73"/>
-      <c r="BH9" s="73"/>
-      <c r="BI9" s="73"/>
-      <c r="BJ9" s="73"/>
+      <c r="BD9" s="77"/>
+      <c r="BE9" s="77"/>
+      <c r="BF9" s="77"/>
+      <c r="BG9" s="77"/>
+      <c r="BH9" s="77"/>
+      <c r="BI9" s="77"/>
+      <c r="BJ9" s="77"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A10" s="16"/>
@@ -2800,9 +2842,9 @@
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="68"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="70"/>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
       <c r="N10" s="24"/>
@@ -2847,13 +2889,13 @@
       <c r="BA10" s="24"/>
       <c r="BB10" s="24"/>
       <c r="BC10" s="24"/>
-      <c r="BD10" s="73"/>
-      <c r="BE10" s="73"/>
-      <c r="BF10" s="73"/>
-      <c r="BG10" s="73"/>
-      <c r="BH10" s="73"/>
-      <c r="BI10" s="73"/>
-      <c r="BJ10" s="73"/>
+      <c r="BD10" s="77"/>
+      <c r="BE10" s="77"/>
+      <c r="BF10" s="77"/>
+      <c r="BG10" s="77"/>
+      <c r="BH10" s="77"/>
+      <c r="BI10" s="77"/>
+      <c r="BJ10" s="77"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A11" s="16"/>
@@ -2887,7 +2929,7 @@
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
       <c r="V11" s="24"/>
-      <c r="W11" s="69"/>
+      <c r="W11" s="72"/>
       <c r="X11" s="24"/>
       <c r="Y11" s="24"/>
       <c r="Z11" s="24"/>
@@ -2920,13 +2962,13 @@
       <c r="BA11" s="24"/>
       <c r="BB11" s="24"/>
       <c r="BC11" s="24"/>
-      <c r="BD11" s="73"/>
-      <c r="BE11" s="73"/>
-      <c r="BF11" s="73"/>
-      <c r="BG11" s="73"/>
-      <c r="BH11" s="73"/>
-      <c r="BI11" s="73"/>
-      <c r="BJ11" s="73"/>
+      <c r="BD11" s="77"/>
+      <c r="BE11" s="77"/>
+      <c r="BF11" s="77"/>
+      <c r="BG11" s="77"/>
+      <c r="BH11" s="77"/>
+      <c r="BI11" s="77"/>
+      <c r="BJ11" s="77"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A12" s="16"/>
@@ -2990,13 +3032,13 @@
       <c r="BA12" s="24"/>
       <c r="BB12" s="24"/>
       <c r="BC12" s="24"/>
-      <c r="BD12" s="73"/>
-      <c r="BE12" s="73"/>
-      <c r="BF12" s="73"/>
-      <c r="BG12" s="73"/>
-      <c r="BH12" s="73"/>
-      <c r="BI12" s="73"/>
-      <c r="BJ12" s="73"/>
+      <c r="BD12" s="77"/>
+      <c r="BE12" s="77"/>
+      <c r="BF12" s="77"/>
+      <c r="BG12" s="77"/>
+      <c r="BH12" s="77"/>
+      <c r="BI12" s="77"/>
+      <c r="BJ12" s="77"/>
     </row>
     <row r="13" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A13" s="16"/>
@@ -3060,30 +3102,23 @@
       <c r="BA13" s="24"/>
       <c r="BB13" s="24"/>
       <c r="BC13" s="24"/>
-      <c r="BD13" s="73"/>
-      <c r="BE13" s="73"/>
-      <c r="BF13" s="73"/>
-      <c r="BG13" s="73"/>
-      <c r="BH13" s="73"/>
-      <c r="BI13" s="73"/>
-      <c r="BJ13" s="73"/>
+      <c r="BD13" s="77"/>
+      <c r="BE13" s="77"/>
+      <c r="BF13" s="77"/>
+      <c r="BG13" s="77"/>
+      <c r="BH13" s="77"/>
+      <c r="BI13" s="77"/>
+      <c r="BJ13" s="77"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A14" s="16"/>
       <c r="B14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="26">
-        <v>45077</v>
-      </c>
-      <c r="D14" s="27">
-        <v>45085</v>
-      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="23">
-        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>9</v>
-      </c>
+      <c r="F14" s="23"/>
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
@@ -3095,23 +3130,23 @@
       <c r="O14" s="24"/>
       <c r="P14" s="24"/>
       <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="71"/>
+      <c r="T14" s="71"/>
       <c r="U14" s="24"/>
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="24"/>
+      <c r="Y14" s="73"/>
+      <c r="Z14" s="73"/>
+      <c r="AA14" s="73"/>
       <c r="AB14" s="24"/>
       <c r="AC14" s="24"/>
       <c r="AD14" s="24"/>
       <c r="AE14" s="24"/>
-      <c r="AF14" s="24"/>
-      <c r="AG14" s="24"/>
-      <c r="AH14" s="24"/>
+      <c r="AF14" s="73"/>
+      <c r="AG14" s="73"/>
+      <c r="AH14" s="73"/>
       <c r="AI14" s="24"/>
       <c r="AJ14" s="24"/>
       <c r="AK14" s="24"/>
@@ -3128,18 +3163,18 @@
       <c r="AV14" s="24"/>
       <c r="AW14" s="24"/>
       <c r="AX14" s="24"/>
-      <c r="AY14" s="24"/>
-      <c r="AZ14" s="24"/>
-      <c r="BA14" s="24"/>
-      <c r="BB14" s="24"/>
-      <c r="BC14" s="24"/>
-      <c r="BD14" s="73"/>
-      <c r="BE14" s="73"/>
-      <c r="BF14" s="73"/>
-      <c r="BG14" s="73"/>
-      <c r="BH14" s="73"/>
-      <c r="BI14" s="73"/>
-      <c r="BJ14" s="73"/>
+      <c r="AY14" s="73"/>
+      <c r="AZ14" s="73"/>
+      <c r="BA14" s="73"/>
+      <c r="BB14" s="73"/>
+      <c r="BC14" s="73"/>
+      <c r="BD14" s="78"/>
+      <c r="BE14" s="78"/>
+      <c r="BF14" s="78"/>
+      <c r="BG14" s="78"/>
+      <c r="BH14" s="77"/>
+      <c r="BI14" s="77"/>
+      <c r="BJ14" s="77"/>
     </row>
     <row r="15" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A15" s="16"/>
@@ -3202,13 +3237,13 @@
       <c r="BA15" s="24"/>
       <c r="BB15" s="24"/>
       <c r="BC15" s="24"/>
-      <c r="BD15" s="73"/>
-      <c r="BE15" s="73"/>
-      <c r="BF15" s="73"/>
-      <c r="BG15" s="73"/>
-      <c r="BH15" s="73"/>
-      <c r="BI15" s="73"/>
-      <c r="BJ15" s="73"/>
+      <c r="BD15" s="77"/>
+      <c r="BE15" s="77"/>
+      <c r="BF15" s="77"/>
+      <c r="BG15" s="77"/>
+      <c r="BH15" s="77"/>
+      <c r="BI15" s="77"/>
+      <c r="BJ15" s="77"/>
     </row>
     <row r="16" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A16" s="16"/>
@@ -3275,13 +3310,13 @@
       <c r="BA16" s="24"/>
       <c r="BB16" s="24"/>
       <c r="BC16" s="24"/>
-      <c r="BD16" s="73"/>
-      <c r="BE16" s="73"/>
-      <c r="BF16" s="73"/>
-      <c r="BG16" s="73"/>
-      <c r="BH16" s="73"/>
-      <c r="BI16" s="73"/>
-      <c r="BJ16" s="73"/>
+      <c r="BD16" s="77"/>
+      <c r="BE16" s="77"/>
+      <c r="BF16" s="77"/>
+      <c r="BG16" s="77"/>
+      <c r="BH16" s="77"/>
+      <c r="BI16" s="77"/>
+      <c r="BJ16" s="77"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A17" s="16"/>
@@ -3292,12 +3327,12 @@
         <v>45041</v>
       </c>
       <c r="D17" s="33">
-        <v>45043</v>
+        <v>45044</v>
       </c>
       <c r="E17" s="23"/>
       <c r="F17" s="23">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
@@ -3311,8 +3346,8 @@
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
-      <c r="S17" s="69"/>
-      <c r="T17" s="69"/>
+      <c r="S17" s="72"/>
+      <c r="T17" s="72"/>
       <c r="U17" s="24"/>
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
@@ -3348,30 +3383,23 @@
       <c r="BA17" s="24"/>
       <c r="BB17" s="24"/>
       <c r="BC17" s="24"/>
-      <c r="BD17" s="73"/>
-      <c r="BE17" s="73"/>
-      <c r="BF17" s="73"/>
-      <c r="BG17" s="73"/>
-      <c r="BH17" s="73"/>
-      <c r="BI17" s="73"/>
-      <c r="BJ17" s="73"/>
+      <c r="BD17" s="77"/>
+      <c r="BE17" s="77"/>
+      <c r="BF17" s="77"/>
+      <c r="BG17" s="77"/>
+      <c r="BH17" s="77"/>
+      <c r="BI17" s="77"/>
+      <c r="BJ17" s="77"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A18" s="16"/>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="32">
-        <v>45041</v>
-      </c>
-      <c r="D18" s="33">
-        <v>45043</v>
-      </c>
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="23"/>
-      <c r="F18" s="23">
-        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>3</v>
-      </c>
+      <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
@@ -3380,7 +3408,7 @@
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
       <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
+      <c r="O18" s="71"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
@@ -3388,7 +3416,7 @@
       <c r="T18" s="24"/>
       <c r="U18" s="24"/>
       <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
+      <c r="W18" s="72"/>
       <c r="X18" s="24"/>
       <c r="Y18" s="24"/>
       <c r="Z18" s="24"/>
@@ -3421,30 +3449,23 @@
       <c r="BA18" s="24"/>
       <c r="BB18" s="24"/>
       <c r="BC18" s="24"/>
-      <c r="BD18" s="73"/>
-      <c r="BE18" s="73"/>
-      <c r="BF18" s="73"/>
-      <c r="BG18" s="73"/>
-      <c r="BH18" s="73"/>
-      <c r="BI18" s="73"/>
-      <c r="BJ18" s="73"/>
+      <c r="BD18" s="77"/>
+      <c r="BE18" s="77"/>
+      <c r="BF18" s="77"/>
+      <c r="BG18" s="77"/>
+      <c r="BH18" s="77"/>
+      <c r="BI18" s="77"/>
+      <c r="BJ18" s="77"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A19" s="16"/>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="32">
-        <v>45043</v>
-      </c>
-      <c r="D19" s="33">
-        <v>45044</v>
-      </c>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="23">
-        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>2</v>
-      </c>
+      <c r="F19" s="23"/>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
@@ -3454,14 +3475,14 @@
       <c r="M19" s="24"/>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
+      <c r="P19" s="71"/>
+      <c r="Q19" s="71"/>
       <c r="R19" s="24"/>
       <c r="S19" s="24"/>
       <c r="T19" s="24"/>
       <c r="U19" s="24"/>
       <c r="V19" s="24"/>
-      <c r="W19" s="69"/>
+      <c r="W19" s="72"/>
       <c r="X19" s="24"/>
       <c r="Y19" s="24"/>
       <c r="Z19" s="24"/>
@@ -3494,25 +3515,21 @@
       <c r="BA19" s="24"/>
       <c r="BB19" s="24"/>
       <c r="BC19" s="24"/>
-      <c r="BD19" s="73"/>
-      <c r="BE19" s="73"/>
-      <c r="BF19" s="73"/>
-      <c r="BG19" s="73"/>
-      <c r="BH19" s="73"/>
-      <c r="BI19" s="73"/>
-      <c r="BJ19" s="73"/>
+      <c r="BD19" s="77"/>
+      <c r="BE19" s="77"/>
+      <c r="BF19" s="77"/>
+      <c r="BG19" s="77"/>
+      <c r="BH19" s="77"/>
+      <c r="BI19" s="77"/>
+      <c r="BJ19" s="77"/>
     </row>
-    <row r="20" s="1" customFormat="1" ht="21" spans="1:62">
+    <row r="20" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A20" s="16"/>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="32">
-        <v>45044</v>
-      </c>
-      <c r="D20" s="33">
-        <v>45044</v>
-      </c>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
       <c r="G20" s="24"/>
@@ -3525,13 +3542,13 @@
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
       <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="68"/>
+      <c r="Q20" s="71"/>
+      <c r="R20" s="71"/>
       <c r="S20" s="24"/>
       <c r="T20" s="24"/>
       <c r="U20" s="24"/>
       <c r="V20" s="24"/>
-      <c r="W20" s="69"/>
+      <c r="W20" s="72"/>
       <c r="X20" s="24"/>
       <c r="Y20" s="24"/>
       <c r="Z20" s="24"/>
@@ -3564,15 +3581,15 @@
       <c r="BA20" s="24"/>
       <c r="BB20" s="24"/>
       <c r="BC20" s="24"/>
-      <c r="BD20" s="73"/>
-      <c r="BE20" s="73"/>
-      <c r="BF20" s="73"/>
-      <c r="BG20" s="73"/>
-      <c r="BH20" s="73"/>
-      <c r="BI20" s="73"/>
-      <c r="BJ20" s="73"/>
+      <c r="BD20" s="77"/>
+      <c r="BE20" s="77"/>
+      <c r="BF20" s="77"/>
+      <c r="BG20" s="77"/>
+      <c r="BH20" s="77"/>
+      <c r="BI20" s="77"/>
+      <c r="BJ20" s="77"/>
     </row>
-    <row r="21" s="1" customFormat="1" ht="21" spans="1:62">
+    <row r="21" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A21" s="16"/>
       <c r="B21" s="31" t="s">
         <v>19</v>
@@ -3581,12 +3598,12 @@
         <v>45044</v>
       </c>
       <c r="D21" s="33">
-        <v>45046</v>
+        <v>45044</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23">
-        <f t="shared" ref="F21:F43" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>3</v>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>1</v>
       </c>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
@@ -3604,7 +3621,7 @@
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
+      <c r="W21" s="72"/>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
       <c r="Z21" s="24"/>
@@ -3637,26 +3654,27 @@
       <c r="BA21" s="24"/>
       <c r="BB21" s="24"/>
       <c r="BC21" s="24"/>
-      <c r="BD21" s="73"/>
-      <c r="BE21" s="73"/>
-      <c r="BF21" s="73"/>
-      <c r="BG21" s="73"/>
-      <c r="BH21" s="73"/>
-      <c r="BI21" s="73"/>
-      <c r="BJ21" s="73"/>
+      <c r="BD21" s="77"/>
+      <c r="BE21" s="77"/>
+      <c r="BF21" s="77"/>
+      <c r="BG21" s="77"/>
+      <c r="BH21" s="77"/>
+      <c r="BI21" s="77"/>
+      <c r="BJ21" s="77"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A22" s="16"/>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="36"/>
+      <c r="C22" s="32">
+        <v>45044</v>
+      </c>
+      <c r="D22" s="33">
+        <v>45044</v>
+      </c>
       <c r="E22" s="23"/>
-      <c r="F22" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="F22" s="23"/>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
@@ -3668,12 +3686,12 @@
       <c r="O22" s="24"/>
       <c r="P22" s="24"/>
       <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
+      <c r="R22" s="70"/>
       <c r="S22" s="24"/>
       <c r="T22" s="24"/>
       <c r="U22" s="24"/>
       <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
+      <c r="W22" s="72"/>
       <c r="X22" s="24"/>
       <c r="Y22" s="24"/>
       <c r="Z22" s="24"/>
@@ -3706,29 +3724,25 @@
       <c r="BA22" s="24"/>
       <c r="BB22" s="24"/>
       <c r="BC22" s="24"/>
-      <c r="BD22" s="73"/>
-      <c r="BE22" s="73"/>
-      <c r="BF22" s="73"/>
-      <c r="BG22" s="73"/>
-      <c r="BH22" s="73"/>
-      <c r="BI22" s="73"/>
-      <c r="BJ22" s="73"/>
+      <c r="BD22" s="77"/>
+      <c r="BE22" s="77"/>
+      <c r="BF22" s="77"/>
+      <c r="BG22" s="77"/>
+      <c r="BH22" s="77"/>
+      <c r="BI22" s="77"/>
+      <c r="BJ22" s="77"/>
     </row>
-    <row r="23" s="1" customFormat="1" ht="21" spans="1:62">
+    <row r="23" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A23" s="16"/>
       <c r="B23" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="38">
-        <v>45046</v>
-      </c>
-      <c r="D23" s="39">
-        <v>45050</v>
-      </c>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="23">
-        <f t="shared" si="5"/>
-        <v>5</v>
+      <c r="F23" s="23" t="str">
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v/>
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
@@ -3779,28 +3793,28 @@
       <c r="BA23" s="24"/>
       <c r="BB23" s="24"/>
       <c r="BC23" s="24"/>
-      <c r="BD23" s="73"/>
-      <c r="BE23" s="73"/>
-      <c r="BF23" s="73"/>
-      <c r="BG23" s="73"/>
-      <c r="BH23" s="73"/>
-      <c r="BI23" s="73"/>
-      <c r="BJ23" s="73"/>
+      <c r="BD23" s="77"/>
+      <c r="BE23" s="77"/>
+      <c r="BF23" s="77"/>
+      <c r="BG23" s="77"/>
+      <c r="BH23" s="77"/>
+      <c r="BI23" s="77"/>
+      <c r="BJ23" s="77"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A24" s="16"/>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="41">
         <v>45046</v>
       </c>
-      <c r="D24" s="39">
+      <c r="D24" s="42">
         <v>45050</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="23">
-        <f t="shared" si="5"/>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>5</v>
       </c>
       <c r="G24" s="24"/>
@@ -3852,30 +3866,23 @@
       <c r="BA24" s="24"/>
       <c r="BB24" s="24"/>
       <c r="BC24" s="24"/>
-      <c r="BD24" s="73"/>
-      <c r="BE24" s="73"/>
-      <c r="BF24" s="73"/>
-      <c r="BG24" s="73"/>
-      <c r="BH24" s="73"/>
-      <c r="BI24" s="73"/>
-      <c r="BJ24" s="73"/>
+      <c r="BD24" s="77"/>
+      <c r="BE24" s="77"/>
+      <c r="BF24" s="77"/>
+      <c r="BG24" s="77"/>
+      <c r="BH24" s="77"/>
+      <c r="BI24" s="77"/>
+      <c r="BJ24" s="77"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A25" s="16"/>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="38">
-        <v>45050</v>
-      </c>
-      <c r="D25" s="39">
-        <v>45051</v>
-      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="36"/>
       <c r="E25" s="23"/>
-      <c r="F25" s="23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
+      <c r="F25" s="23"/>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
@@ -3889,9 +3896,9 @@
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
       <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
+      <c r="T25" s="71"/>
+      <c r="U25" s="71"/>
+      <c r="V25" s="71"/>
       <c r="W25" s="24"/>
       <c r="X25" s="24"/>
       <c r="Y25" s="24"/>
@@ -3925,30 +3932,23 @@
       <c r="BA25" s="24"/>
       <c r="BB25" s="24"/>
       <c r="BC25" s="24"/>
-      <c r="BD25" s="73"/>
-      <c r="BE25" s="73"/>
-      <c r="BF25" s="73"/>
-      <c r="BG25" s="73"/>
-      <c r="BH25" s="73"/>
-      <c r="BI25" s="73"/>
-      <c r="BJ25" s="73"/>
+      <c r="BD25" s="77"/>
+      <c r="BE25" s="77"/>
+      <c r="BF25" s="77"/>
+      <c r="BG25" s="77"/>
+      <c r="BH25" s="77"/>
+      <c r="BI25" s="77"/>
+      <c r="BJ25" s="77"/>
     </row>
-    <row r="26" s="1" customFormat="1" ht="21" spans="1:62">
+    <row r="26" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A26" s="16"/>
-      <c r="B26" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="38">
-        <v>45051</v>
-      </c>
-      <c r="D26" s="39">
-        <v>45051</v>
-      </c>
+      <c r="B26" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
       <c r="E26" s="23"/>
-      <c r="F26" s="23">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
+      <c r="F26" s="23"/>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
       <c r="I26" s="24"/>
@@ -3965,8 +3965,8 @@
       <c r="T26" s="24"/>
       <c r="U26" s="24"/>
       <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
+      <c r="W26" s="71"/>
+      <c r="X26" s="71"/>
       <c r="Y26" s="24"/>
       <c r="Z26" s="24"/>
       <c r="AA26" s="24"/>
@@ -3998,29 +3998,29 @@
       <c r="BA26" s="24"/>
       <c r="BB26" s="24"/>
       <c r="BC26" s="24"/>
-      <c r="BD26" s="73"/>
-      <c r="BE26" s="73"/>
-      <c r="BF26" s="73"/>
-      <c r="BG26" s="73"/>
-      <c r="BH26" s="73"/>
-      <c r="BI26" s="73"/>
-      <c r="BJ26" s="73"/>
+      <c r="BD26" s="77"/>
+      <c r="BE26" s="77"/>
+      <c r="BF26" s="77"/>
+      <c r="BG26" s="77"/>
+      <c r="BH26" s="77"/>
+      <c r="BI26" s="77"/>
+      <c r="BJ26" s="77"/>
     </row>
-    <row r="27" s="1" customFormat="1" ht="21" spans="1:62">
+    <row r="27" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A27" s="16"/>
-      <c r="B27" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="38">
+      <c r="B27" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="41">
+        <v>45050</v>
+      </c>
+      <c r="D27" s="42">
         <v>45051</v>
-      </c>
-      <c r="D27" s="39">
-        <v>45053</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="23">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>2</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
@@ -4071,25 +4071,29 @@
       <c r="BA27" s="24"/>
       <c r="BB27" s="24"/>
       <c r="BC27" s="24"/>
-      <c r="BD27" s="73"/>
-      <c r="BE27" s="73"/>
-      <c r="BF27" s="73"/>
-      <c r="BG27" s="73"/>
-      <c r="BH27" s="73"/>
-      <c r="BI27" s="73"/>
-      <c r="BJ27" s="73"/>
+      <c r="BD27" s="77"/>
+      <c r="BE27" s="77"/>
+      <c r="BF27" s="77"/>
+      <c r="BG27" s="77"/>
+      <c r="BH27" s="77"/>
+      <c r="BI27" s="77"/>
+      <c r="BJ27" s="77"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A28" s="16"/>
       <c r="B28" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
+        <v>20</v>
+      </c>
+      <c r="C28" s="41">
+        <v>45051</v>
+      </c>
+      <c r="D28" s="42">
+        <v>45051</v>
+      </c>
       <c r="E28" s="23"/>
-      <c r="F28" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+      <c r="F28" s="23">
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>1</v>
       </c>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
@@ -4140,29 +4144,25 @@
       <c r="BA28" s="24"/>
       <c r="BB28" s="24"/>
       <c r="BC28" s="24"/>
-      <c r="BD28" s="73"/>
-      <c r="BE28" s="73"/>
-      <c r="BF28" s="73"/>
-      <c r="BG28" s="73"/>
-      <c r="BH28" s="73"/>
-      <c r="BI28" s="73"/>
-      <c r="BJ28" s="73"/>
+      <c r="BD28" s="77"/>
+      <c r="BE28" s="77"/>
+      <c r="BF28" s="77"/>
+      <c r="BG28" s="77"/>
+      <c r="BH28" s="77"/>
+      <c r="BI28" s="77"/>
+      <c r="BJ28" s="77"/>
     </row>
-    <row r="29" s="1" customFormat="1" ht="27" customHeight="1" spans="1:62">
+    <row r="29" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A29" s="16"/>
       <c r="B29" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="44">
-        <v>45053</v>
-      </c>
-      <c r="D29" s="45">
-        <v>45057</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C29" s="44"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="23"/>
-      <c r="F29" s="23">
-        <f t="shared" si="5"/>
-        <v>5</v>
+      <c r="F29" s="23" t="str">
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v/>
       </c>
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
@@ -4213,28 +4213,28 @@
       <c r="BA29" s="24"/>
       <c r="BB29" s="24"/>
       <c r="BC29" s="24"/>
-      <c r="BD29" s="73"/>
-      <c r="BE29" s="73"/>
-      <c r="BF29" s="73"/>
-      <c r="BG29" s="73"/>
-      <c r="BH29" s="73"/>
-      <c r="BI29" s="73"/>
-      <c r="BJ29" s="73"/>
+      <c r="BD29" s="77"/>
+      <c r="BE29" s="77"/>
+      <c r="BF29" s="77"/>
+      <c r="BG29" s="77"/>
+      <c r="BH29" s="77"/>
+      <c r="BI29" s="77"/>
+      <c r="BJ29" s="77"/>
     </row>
-    <row r="30" s="1" customFormat="1" ht="21.75" spans="1:62">
+    <row r="30" s="1" customFormat="1" ht="27" customHeight="1" spans="1:62">
       <c r="A30" s="16"/>
-      <c r="B30" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="44">
+      <c r="B30" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="47">
         <v>45053</v>
       </c>
-      <c r="D30" s="45">
+      <c r="D30" s="48">
         <v>45057</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="23">
-        <f t="shared" si="5"/>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>5</v>
       </c>
       <c r="G30" s="24"/>
@@ -4286,30 +4286,23 @@
       <c r="BA30" s="24"/>
       <c r="BB30" s="24"/>
       <c r="BC30" s="24"/>
-      <c r="BD30" s="73"/>
-      <c r="BE30" s="73"/>
-      <c r="BF30" s="73"/>
-      <c r="BG30" s="73"/>
-      <c r="BH30" s="73"/>
-      <c r="BI30" s="73"/>
-      <c r="BJ30" s="73"/>
+      <c r="BD30" s="77"/>
+      <c r="BE30" s="77"/>
+      <c r="BF30" s="77"/>
+      <c r="BG30" s="77"/>
+      <c r="BH30" s="77"/>
+      <c r="BI30" s="77"/>
+      <c r="BJ30" s="77"/>
     </row>
     <row r="31" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A31" s="16"/>
-      <c r="B31" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="44">
-        <v>45057</v>
-      </c>
-      <c r="D31" s="45">
-        <v>45058</v>
-      </c>
+      <c r="B31" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="35"/>
+      <c r="D31" s="36"/>
       <c r="E31" s="23"/>
-      <c r="F31" s="23">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
+      <c r="F31" s="23"/>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
       <c r="I31" s="24"/>
@@ -4359,29 +4352,29 @@
       <c r="BA31" s="24"/>
       <c r="BB31" s="24"/>
       <c r="BC31" s="24"/>
-      <c r="BD31" s="73"/>
-      <c r="BE31" s="73"/>
-      <c r="BF31" s="73"/>
-      <c r="BG31" s="73"/>
-      <c r="BH31" s="73"/>
-      <c r="BI31" s="73"/>
-      <c r="BJ31" s="73"/>
+      <c r="BD31" s="77"/>
+      <c r="BE31" s="77"/>
+      <c r="BF31" s="77"/>
+      <c r="BG31" s="77"/>
+      <c r="BH31" s="77"/>
+      <c r="BI31" s="77"/>
+      <c r="BJ31" s="77"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A32" s="16"/>
-      <c r="B32" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="44">
-        <v>45058</v>
-      </c>
-      <c r="D32" s="45">
+      <c r="B32" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="47">
+        <v>45057</v>
+      </c>
+      <c r="D32" s="48">
         <v>45058</v>
       </c>
       <c r="E32" s="23"/>
       <c r="F32" s="23">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>2</v>
       </c>
       <c r="G32" s="24"/>
       <c r="H32" s="24"/>
@@ -4432,29 +4425,29 @@
       <c r="BA32" s="24"/>
       <c r="BB32" s="24"/>
       <c r="BC32" s="24"/>
-      <c r="BD32" s="73"/>
-      <c r="BE32" s="73"/>
-      <c r="BF32" s="73"/>
-      <c r="BG32" s="73"/>
-      <c r="BH32" s="73"/>
-      <c r="BI32" s="73"/>
-      <c r="BJ32" s="73"/>
+      <c r="BD32" s="77"/>
+      <c r="BE32" s="77"/>
+      <c r="BF32" s="77"/>
+      <c r="BG32" s="77"/>
+      <c r="BH32" s="77"/>
+      <c r="BI32" s="77"/>
+      <c r="BJ32" s="77"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A33" s="16"/>
-      <c r="B33" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="44">
+      <c r="B33" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="47">
         <v>45058</v>
       </c>
-      <c r="D33" s="45">
-        <v>45060</v>
+      <c r="D33" s="48">
+        <v>45058</v>
       </c>
       <c r="E33" s="23"/>
       <c r="F33" s="23">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>1</v>
       </c>
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
@@ -4505,24 +4498,24 @@
       <c r="BA33" s="24"/>
       <c r="BB33" s="24"/>
       <c r="BC33" s="24"/>
-      <c r="BD33" s="73"/>
-      <c r="BE33" s="73"/>
-      <c r="BF33" s="73"/>
-      <c r="BG33" s="73"/>
-      <c r="BH33" s="73"/>
-      <c r="BI33" s="73"/>
-      <c r="BJ33" s="73"/>
+      <c r="BD33" s="77"/>
+      <c r="BE33" s="77"/>
+      <c r="BF33" s="77"/>
+      <c r="BG33" s="77"/>
+      <c r="BH33" s="77"/>
+      <c r="BI33" s="77"/>
+      <c r="BJ33" s="77"/>
     </row>
-    <row r="34" s="1" customFormat="1" ht="21.75" spans="1:62">
+    <row r="34" s="1" customFormat="1" ht="21" spans="1:62">
       <c r="A34" s="16"/>
-      <c r="B34" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="47"/>
-      <c r="D34" s="48"/>
+      <c r="B34" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="50"/>
+      <c r="D34" s="51"/>
       <c r="E34" s="23"/>
       <c r="F34" s="23" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="G34" s="24"/>
@@ -4574,29 +4567,29 @@
       <c r="BA34" s="24"/>
       <c r="BB34" s="24"/>
       <c r="BC34" s="24"/>
-      <c r="BD34" s="73"/>
-      <c r="BE34" s="73"/>
-      <c r="BF34" s="73"/>
-      <c r="BG34" s="73"/>
-      <c r="BH34" s="73"/>
-      <c r="BI34" s="73"/>
-      <c r="BJ34" s="73"/>
+      <c r="BD34" s="77"/>
+      <c r="BE34" s="77"/>
+      <c r="BF34" s="77"/>
+      <c r="BG34" s="77"/>
+      <c r="BH34" s="77"/>
+      <c r="BI34" s="77"/>
+      <c r="BJ34" s="77"/>
     </row>
-    <row r="35" s="1" customFormat="1" ht="21" spans="1:62">
+    <row r="35" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A35" s="16"/>
-      <c r="B35" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="50">
+      <c r="B35" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="53">
         <v>45060</v>
       </c>
-      <c r="D35" s="51">
-        <v>45063</v>
+      <c r="D35" s="54">
+        <v>45077</v>
       </c>
       <c r="E35" s="23"/>
       <c r="F35" s="23">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>18</v>
       </c>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
@@ -4647,30 +4640,23 @@
       <c r="BA35" s="24"/>
       <c r="BB35" s="24"/>
       <c r="BC35" s="24"/>
-      <c r="BD35" s="73"/>
-      <c r="BE35" s="73"/>
-      <c r="BF35" s="73"/>
-      <c r="BG35" s="73"/>
-      <c r="BH35" s="73"/>
-      <c r="BI35" s="73"/>
-      <c r="BJ35" s="73"/>
+      <c r="BD35" s="77"/>
+      <c r="BE35" s="77"/>
+      <c r="BF35" s="77"/>
+      <c r="BG35" s="77"/>
+      <c r="BH35" s="77"/>
+      <c r="BI35" s="77"/>
+      <c r="BJ35" s="77"/>
     </row>
     <row r="36" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A36" s="16"/>
-      <c r="B36" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="50">
-        <v>45063</v>
-      </c>
-      <c r="D36" s="51">
-        <v>45077</v>
-      </c>
+      <c r="B36" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="35"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="23"/>
-      <c r="F36" s="23">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
+      <c r="F36" s="23"/>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
       <c r="I36" s="24"/>
@@ -4698,16 +4684,16 @@
       <c r="AE36" s="24"/>
       <c r="AF36" s="24"/>
       <c r="AG36" s="24"/>
-      <c r="AH36" s="24"/>
-      <c r="AI36" s="24"/>
-      <c r="AJ36" s="24"/>
-      <c r="AK36" s="24"/>
-      <c r="AL36" s="24"/>
-      <c r="AM36" s="24"/>
-      <c r="AN36" s="24"/>
-      <c r="AO36" s="24"/>
-      <c r="AP36" s="24"/>
-      <c r="AQ36" s="24"/>
+      <c r="AH36" s="71"/>
+      <c r="AI36" s="71"/>
+      <c r="AJ36" s="71"/>
+      <c r="AK36" s="71"/>
+      <c r="AL36" s="71"/>
+      <c r="AM36" s="71"/>
+      <c r="AN36" s="71"/>
+      <c r="AO36" s="71"/>
+      <c r="AP36" s="71"/>
+      <c r="AQ36" s="71"/>
       <c r="AR36" s="24"/>
       <c r="AS36" s="24"/>
       <c r="AT36" s="24"/>
@@ -4720,30 +4706,23 @@
       <c r="BA36" s="24"/>
       <c r="BB36" s="24"/>
       <c r="BC36" s="24"/>
-      <c r="BD36" s="73"/>
-      <c r="BE36" s="73"/>
-      <c r="BF36" s="73"/>
-      <c r="BG36" s="73"/>
-      <c r="BH36" s="73"/>
-      <c r="BI36" s="73"/>
-      <c r="BJ36" s="73"/>
+      <c r="BD36" s="77"/>
+      <c r="BE36" s="77"/>
+      <c r="BF36" s="77"/>
+      <c r="BG36" s="77"/>
+      <c r="BH36" s="77"/>
+      <c r="BI36" s="77"/>
+      <c r="BJ36" s="77"/>
     </row>
     <row r="37" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A37" s="16"/>
-      <c r="B37" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="50">
-        <v>45072</v>
-      </c>
-      <c r="D37" s="51">
-        <v>45077</v>
-      </c>
+      <c r="B37" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="35"/>
+      <c r="D37" s="36"/>
       <c r="E37" s="23"/>
-      <c r="F37" s="23">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
+      <c r="F37" s="23"/>
       <c r="G37" s="24"/>
       <c r="H37" s="24"/>
       <c r="I37" s="24"/>
@@ -4781,35 +4760,41 @@
       <c r="AO37" s="24"/>
       <c r="AP37" s="24"/>
       <c r="AQ37" s="24"/>
-      <c r="AR37" s="24"/>
-      <c r="AS37" s="24"/>
-      <c r="AT37" s="24"/>
-      <c r="AU37" s="24"/>
-      <c r="AV37" s="24"/>
-      <c r="AW37" s="24"/>
-      <c r="AX37" s="24"/>
-      <c r="AY37" s="24"/>
+      <c r="AR37" s="71"/>
+      <c r="AS37" s="71"/>
+      <c r="AT37" s="71"/>
+      <c r="AU37" s="71"/>
+      <c r="AV37" s="71"/>
+      <c r="AW37" s="71"/>
+      <c r="AX37" s="71"/>
+      <c r="AY37" s="71"/>
       <c r="AZ37" s="24"/>
       <c r="BA37" s="24"/>
       <c r="BB37" s="24"/>
       <c r="BC37" s="24"/>
-      <c r="BD37" s="73"/>
-      <c r="BE37" s="73"/>
-      <c r="BF37" s="73"/>
-      <c r="BG37" s="73"/>
-      <c r="BH37" s="73"/>
-      <c r="BI37" s="73"/>
-      <c r="BJ37" s="73"/>
+      <c r="BD37" s="77"/>
+      <c r="BE37" s="77"/>
+      <c r="BF37" s="77"/>
+      <c r="BG37" s="77"/>
+      <c r="BH37" s="77"/>
+      <c r="BI37" s="77"/>
+      <c r="BJ37" s="77"/>
     </row>
     <row r="38" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A38" s="16"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="54"/>
+      <c r="B38" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="53">
+        <v>45072</v>
+      </c>
+      <c r="D38" s="54">
+        <v>45077</v>
+      </c>
       <c r="E38" s="23"/>
-      <c r="F38" s="23" t="str">
-        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v/>
+      <c r="F38" s="23">
+        <f t="shared" ref="F38:F44" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>6</v>
       </c>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
@@ -4860,19 +4845,19 @@
       <c r="BA38" s="24"/>
       <c r="BB38" s="24"/>
       <c r="BC38" s="24"/>
-      <c r="BD38" s="73"/>
-      <c r="BE38" s="73"/>
-      <c r="BF38" s="73"/>
-      <c r="BG38" s="73"/>
-      <c r="BH38" s="73"/>
-      <c r="BI38" s="73"/>
-      <c r="BJ38" s="73"/>
+      <c r="BD38" s="77"/>
+      <c r="BE38" s="77"/>
+      <c r="BF38" s="77"/>
+      <c r="BG38" s="77"/>
+      <c r="BH38" s="77"/>
+      <c r="BI38" s="77"/>
+      <c r="BJ38" s="77"/>
     </row>
     <row r="39" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A39" s="16"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="54"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="57"/>
       <c r="E39" s="23"/>
       <c r="F39" s="23" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -4927,19 +4912,19 @@
       <c r="BA39" s="24"/>
       <c r="BB39" s="24"/>
       <c r="BC39" s="24"/>
-      <c r="BD39" s="73"/>
-      <c r="BE39" s="73"/>
-      <c r="BF39" s="73"/>
-      <c r="BG39" s="73"/>
-      <c r="BH39" s="73"/>
-      <c r="BI39" s="73"/>
-      <c r="BJ39" s="73"/>
+      <c r="BD39" s="77"/>
+      <c r="BE39" s="77"/>
+      <c r="BF39" s="77"/>
+      <c r="BG39" s="77"/>
+      <c r="BH39" s="77"/>
+      <c r="BI39" s="77"/>
+      <c r="BJ39" s="77"/>
     </row>
     <row r="40" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A40" s="16"/>
-      <c r="B40" s="52"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="54"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="57"/>
       <c r="E40" s="23"/>
       <c r="F40" s="23" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -4994,145 +4979,156 @@
       <c r="BA40" s="24"/>
       <c r="BB40" s="24"/>
       <c r="BC40" s="24"/>
-      <c r="BD40" s="73"/>
-      <c r="BE40" s="73"/>
-      <c r="BF40" s="73"/>
-      <c r="BG40" s="73"/>
-      <c r="BH40" s="73"/>
-      <c r="BI40" s="73"/>
-      <c r="BJ40" s="73"/>
+      <c r="BD40" s="77"/>
+      <c r="BE40" s="77"/>
+      <c r="BF40" s="77"/>
+      <c r="BG40" s="77"/>
+      <c r="BH40" s="77"/>
+      <c r="BI40" s="77"/>
+      <c r="BJ40" s="77"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A41" s="16"/>
-      <c r="B41" s="55" t="s">
-        <v>32</v>
-      </c>
+      <c r="B41" s="55"/>
       <c r="C41" s="56"/>
       <c r="D41" s="57"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58" t="str">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="59"/>
-      <c r="K41" s="59"/>
-      <c r="L41" s="59"/>
-      <c r="M41" s="59"/>
-      <c r="N41" s="59"/>
-      <c r="O41" s="59"/>
-      <c r="P41" s="59"/>
-      <c r="Q41" s="59"/>
-      <c r="R41" s="59"/>
-      <c r="S41" s="59"/>
-      <c r="T41" s="59"/>
-      <c r="U41" s="59"/>
-      <c r="V41" s="59"/>
-      <c r="W41" s="59"/>
-      <c r="X41" s="59"/>
-      <c r="Y41" s="59"/>
-      <c r="Z41" s="59"/>
-      <c r="AA41" s="59"/>
-      <c r="AB41" s="59"/>
-      <c r="AC41" s="59"/>
-      <c r="AD41" s="59"/>
-      <c r="AE41" s="59"/>
-      <c r="AF41" s="59"/>
-      <c r="AG41" s="59"/>
-      <c r="AH41" s="59"/>
-      <c r="AI41" s="59"/>
-      <c r="AJ41" s="59"/>
-      <c r="AK41" s="59"/>
-      <c r="AL41" s="59"/>
-      <c r="AM41" s="59"/>
-      <c r="AN41" s="59"/>
-      <c r="AO41" s="59"/>
-      <c r="AP41" s="59"/>
-      <c r="AQ41" s="59"/>
-      <c r="AR41" s="59"/>
-      <c r="AS41" s="59"/>
-      <c r="AT41" s="59"/>
-      <c r="AU41" s="59"/>
-      <c r="AV41" s="59"/>
-      <c r="AW41" s="59"/>
-      <c r="AX41" s="59"/>
-      <c r="AY41" s="59"/>
-      <c r="AZ41" s="59"/>
-      <c r="BA41" s="59"/>
-      <c r="BB41" s="59"/>
-      <c r="BC41" s="59"/>
-      <c r="BD41" s="74"/>
-      <c r="BE41" s="74"/>
-      <c r="BF41" s="74"/>
-      <c r="BG41" s="74"/>
-      <c r="BH41" s="74"/>
-      <c r="BI41" s="74"/>
-      <c r="BJ41" s="74"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="24"/>
+      <c r="T41" s="24"/>
+      <c r="U41" s="24"/>
+      <c r="V41" s="24"/>
+      <c r="W41" s="24"/>
+      <c r="X41" s="24"/>
+      <c r="Y41" s="24"/>
+      <c r="Z41" s="24"/>
+      <c r="AA41" s="24"/>
+      <c r="AB41" s="24"/>
+      <c r="AC41" s="24"/>
+      <c r="AD41" s="24"/>
+      <c r="AE41" s="24"/>
+      <c r="AF41" s="24"/>
+      <c r="AG41" s="24"/>
+      <c r="AH41" s="24"/>
+      <c r="AI41" s="24"/>
+      <c r="AJ41" s="24"/>
+      <c r="AK41" s="24"/>
+      <c r="AL41" s="24"/>
+      <c r="AM41" s="24"/>
+      <c r="AN41" s="24"/>
+      <c r="AO41" s="24"/>
+      <c r="AP41" s="24"/>
+      <c r="AQ41" s="24"/>
+      <c r="AR41" s="24"/>
+      <c r="AS41" s="24"/>
+      <c r="AT41" s="24"/>
+      <c r="AU41" s="24"/>
+      <c r="AV41" s="24"/>
+      <c r="AW41" s="24"/>
+      <c r="AX41" s="24"/>
+      <c r="AY41" s="24"/>
+      <c r="AZ41" s="24"/>
+      <c r="BA41" s="24"/>
+      <c r="BB41" s="24"/>
+      <c r="BC41" s="24"/>
+      <c r="BD41" s="77"/>
+      <c r="BE41" s="77"/>
+      <c r="BF41" s="77"/>
+      <c r="BG41" s="77"/>
+      <c r="BH41" s="77"/>
+      <c r="BI41" s="77"/>
+      <c r="BJ41" s="77"/>
     </row>
-    <row r="42" spans="1:55">
-      <c r="A42" s="11"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="7"/>
-      <c r="U42" s="7"/>
-      <c r="V42" s="7"/>
-      <c r="W42" s="7"/>
-      <c r="X42" s="7"/>
-      <c r="Y42" s="7"/>
-      <c r="Z42" s="7"/>
-      <c r="AA42" s="7"/>
-      <c r="AB42" s="7"/>
-      <c r="AC42" s="7"/>
-      <c r="AD42" s="7"/>
-      <c r="AE42" s="7"/>
-      <c r="AF42" s="7"/>
-      <c r="AG42" s="7"/>
-      <c r="AH42" s="7"/>
-      <c r="AI42" s="7"/>
-      <c r="AJ42" s="7"/>
-      <c r="AK42" s="7"/>
-      <c r="AL42" s="7"/>
-      <c r="AM42" s="7"/>
-      <c r="AN42" s="7"/>
-      <c r="AO42" s="7"/>
-      <c r="AP42" s="7"/>
-      <c r="AQ42" s="7"/>
-      <c r="AR42" s="7"/>
-      <c r="AS42" s="7"/>
-      <c r="AT42" s="7"/>
-      <c r="AU42" s="7"/>
-      <c r="AV42" s="7"/>
-      <c r="AW42" s="7"/>
-      <c r="AX42" s="7"/>
-      <c r="AY42" s="7"/>
-      <c r="AZ42" s="7"/>
-      <c r="BA42" s="7"/>
-      <c r="BB42" s="7"/>
-      <c r="BC42" s="7"/>
+    <row r="42" s="1" customFormat="1" ht="21.75" spans="1:62">
+      <c r="A42" s="16"/>
+      <c r="B42" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="59"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61" t="str">
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v/>
+      </c>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="62"/>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="62"/>
+      <c r="R42" s="62"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
+      <c r="U42" s="62"/>
+      <c r="V42" s="62"/>
+      <c r="W42" s="62"/>
+      <c r="X42" s="62"/>
+      <c r="Y42" s="62"/>
+      <c r="Z42" s="62"/>
+      <c r="AA42" s="62"/>
+      <c r="AB42" s="62"/>
+      <c r="AC42" s="62"/>
+      <c r="AD42" s="62"/>
+      <c r="AE42" s="62"/>
+      <c r="AF42" s="62"/>
+      <c r="AG42" s="62"/>
+      <c r="AH42" s="62"/>
+      <c r="AI42" s="62"/>
+      <c r="AJ42" s="62"/>
+      <c r="AK42" s="62"/>
+      <c r="AL42" s="62"/>
+      <c r="AM42" s="62"/>
+      <c r="AN42" s="62"/>
+      <c r="AO42" s="62"/>
+      <c r="AP42" s="62"/>
+      <c r="AQ42" s="62"/>
+      <c r="AR42" s="62"/>
+      <c r="AS42" s="62"/>
+      <c r="AT42" s="62"/>
+      <c r="AU42" s="62"/>
+      <c r="AV42" s="62"/>
+      <c r="AW42" s="62"/>
+      <c r="AX42" s="62"/>
+      <c r="AY42" s="62"/>
+      <c r="AZ42" s="62"/>
+      <c r="BA42" s="62"/>
+      <c r="BB42" s="62"/>
+      <c r="BC42" s="62"/>
+      <c r="BD42" s="79"/>
+      <c r="BE42" s="79"/>
+      <c r="BF42" s="79"/>
+      <c r="BG42" s="79"/>
+      <c r="BH42" s="79"/>
+      <c r="BI42" s="79"/>
+      <c r="BJ42" s="79"/>
     </row>
-    <row r="43" spans="2:55">
-      <c r="B43" s="60"/>
+    <row r="43" spans="1:55">
+      <c r="A43" s="11"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="12"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="13"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -5185,9 +5181,9 @@
       <c r="BC43" s="7"/>
     </row>
     <row r="44" spans="2:55">
-      <c r="B44" s="62"/>
+      <c r="B44" s="63"/>
       <c r="C44" s="12"/>
-      <c r="D44" s="7"/>
+      <c r="D44" s="64"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
@@ -5241,7 +5237,7 @@
       <c r="BC44" s="7"/>
     </row>
     <row r="45" spans="2:55">
-      <c r="B45" s="63"/>
+      <c r="B45" s="65"/>
       <c r="C45" s="12"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -5297,7 +5293,7 @@
       <c r="BC45" s="7"/>
     </row>
     <row r="46" spans="2:55">
-      <c r="B46" s="7"/>
+      <c r="B46" s="66"/>
       <c r="C46" s="12"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -5856,6 +5852,62 @@
       <c r="BB55" s="7"/>
       <c r="BC55" s="7"/>
     </row>
+    <row r="56" spans="2:55">
+      <c r="B56" s="7"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
+      <c r="V56" s="7"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="7"/>
+      <c r="Y56" s="7"/>
+      <c r="Z56" s="7"/>
+      <c r="AA56" s="7"/>
+      <c r="AB56" s="7"/>
+      <c r="AC56" s="7"/>
+      <c r="AD56" s="7"/>
+      <c r="AE56" s="7"/>
+      <c r="AF56" s="7"/>
+      <c r="AG56" s="7"/>
+      <c r="AH56" s="7"/>
+      <c r="AI56" s="7"/>
+      <c r="AJ56" s="7"/>
+      <c r="AK56" s="7"/>
+      <c r="AL56" s="7"/>
+      <c r="AM56" s="7"/>
+      <c r="AN56" s="7"/>
+      <c r="AO56" s="7"/>
+      <c r="AP56" s="7"/>
+      <c r="AQ56" s="7"/>
+      <c r="AR56" s="7"/>
+      <c r="AS56" s="7"/>
+      <c r="AT56" s="7"/>
+      <c r="AU56" s="7"/>
+      <c r="AV56" s="7"/>
+      <c r="AW56" s="7"/>
+      <c r="AX56" s="7"/>
+      <c r="AY56" s="7"/>
+      <c r="AZ56" s="7"/>
+      <c r="BA56" s="7"/>
+      <c r="BB56" s="7"/>
+      <c r="BC56" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="B1:BJ1"/>
@@ -5870,12 +5922,12 @@
     <mergeCell ref="AW4:BC4"/>
     <mergeCell ref="BD4:BJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="G5:BJ41">
+  <conditionalFormatting sqref="G5:BJ42">
     <cfRule type="expression" dxfId="0" priority="27">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:BJ41">
+  <conditionalFormatting sqref="G7:BJ42">
     <cfRule type="expression" dxfId="1" priority="25">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Correcciones varias, comprobador Url Serial hecho
-Ortografia, Planificacion, documento
-Reestructuracion del apartado serializacion
-Correccion en los codigo de serializacion para explicar mas facil
</commit_message>
<xml_diff>
--- a/001-Planificacion Diagrama de gant ( plantilla wpsoficce).xlsx
+++ b/001-Planificacion Diagrama de gant ( plantilla wpsoficce).xlsx
@@ -75,19 +75,19 @@
     <t>DAYS</t>
   </si>
   <si>
-    <t>Planificacion Pbl</t>
+    <t>Planificación Pbl</t>
   </si>
   <si>
-    <t>Buscar informacion de RMI</t>
+    <t>Buscar información de RMI</t>
   </si>
   <si>
-    <t>Estructurar informacion Buscada</t>
+    <t>Estructurar información buscada</t>
   </si>
   <si>
-    <t>Reunion inicial</t>
+    <t>Reunión inicial</t>
   </si>
   <si>
-    <t>Etapa de formacion</t>
+    <t>Etapa de formación</t>
   </si>
   <si>
     <t>Ejercicio de proyecto completo</t>
@@ -96,13 +96,13 @@
     <t>Ajustes y correcciones</t>
   </si>
   <si>
-    <t>Apartado basico ( entrada, stub-skeleton, naming server, serializacion)</t>
+    <t>Apartado básico ( entrada, stub-skeleton, naming server, serialización)</t>
   </si>
   <si>
-    <t>Hacer apartado entrada - Documentacion</t>
+    <t>Hacer apartado entrada - Documentación</t>
   </si>
   <si>
-    <t>Apartado basico - ejercicios (plantear, codificar)</t>
+    <t>Apartado básico - ejercicios (plantear, codificar)</t>
   </si>
   <si>
     <t>Ejercicio de stub-skeleton 2</t>
@@ -111,13 +111,13 @@
     <t>Ejercicios de naming server 3-4</t>
   </si>
   <si>
-    <t>Ejercicios de serializacion 3</t>
+    <t>Ejercicios de serialización 3</t>
   </si>
   <si>
-    <t>Apartado basico - Documentacion</t>
+    <t>Apartado básico - Documentación</t>
   </si>
   <si>
-    <t>Reunion segimiento</t>
+    <t>Reunión segimiento</t>
   </si>
   <si>
     <t xml:space="preserve">Apartado de seguridad </t>
@@ -129,25 +129,25 @@
     <t>Ejercicios de buscar Vulnerabilidades  2</t>
   </si>
   <si>
-    <t>Ejercicios  de securizar la aplicacion 1-2 (con RMISecurity manager)</t>
+    <t>Ejercicios  de securizar la aplicación 1-2 (con RMISecurity manager)</t>
   </si>
   <si>
-    <t>Apartado de seguridad- Documentacion</t>
+    <t>Apartado de seguridad- Documentación</t>
   </si>
   <si>
-    <t>Apartado de carga dinamica</t>
+    <t>Apartado de carga dinámica</t>
   </si>
   <si>
-    <t>Apartado Carga dinamica-ejercicios (plantear ,codificar)</t>
+    <t>Apartado Carga dinámica-ejercicios (plantear ,codificar)</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Ejercicios de cálculo distribuido con Rmi 3-4</t>
   </si>
   <si>
-    <t>Carga dinamica- documentacion</t>
+    <t>Carga dinámica- documentación</t>
   </si>
   <si>
-    <t xml:space="preserve">Ejercicios complejos </t>
+    <t xml:space="preserve">Ejercicios completos </t>
   </si>
   <si>
     <t>Ejercicio completo-ejercicios (plantear, codificar)</t>
@@ -156,10 +156,10 @@
     <t>Ejercicio Objetos remotos y seguridad ( repartidores)</t>
   </si>
   <si>
-    <t>Ejercicio carga dinamica ( procesador calculos /finanzas?)</t>
+    <t>Ejercicio carga dinamica (Juego de la vida con Rmi ?)</t>
   </si>
   <si>
-    <t>Ejercicio completo - documentacion</t>
+    <t>Ejercicio completo - documentación</t>
   </si>
   <si>
     <t>Insert new rows ABOVE this one</t>
@@ -170,14 +170,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="182" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="183" formatCode="d"/>
+    <numFmt numFmtId="180" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="181" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="182" formatCode="d"/>
+    <numFmt numFmtId="183" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="38">
     <font>
@@ -289,6 +289,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -298,14 +312,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,18 +349,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -373,16 +395,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,15 +410,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,14 +420,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,7 +443,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,6 +524,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE4DFEC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -560,25 +566,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,31 +596,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -638,13 +626,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,31 +662,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -833,6 +839,36 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -843,6 +879,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -871,45 +916,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -923,16 +929,16 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -942,132 +948,132 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1079,20 +1085,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1104,10 +1110,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1125,10 +1131,10 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,115 +1146,118 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="11" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="11" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="9" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="9" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1257,31 +1266,31 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="181" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1290,22 +1299,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="183" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="15" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="15" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1564,16 +1573,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
-      <color rgb="00B8CCE4"/>
       <color rgb="004A6F9C"/>
       <color rgb="00F9EEEE"/>
       <color rgb="00F2DCDB"/>
       <color rgb="00F8EBEB"/>
       <color rgb="00F9FBF4"/>
       <color rgb="00FFFFFF"/>
-      <color rgb="0044678E"/>
       <color rgb="00E8EEF4"/>
       <color rgb="00F7FAFC"/>
+      <color rgb="0044678E"/>
+      <color rgb="00E4DFEC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1849,7 +1858,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2065,7 +2074,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
-      <c r="M4" s="67"/>
+      <c r="M4" s="68"/>
       <c r="N4" s="9">
         <f>N5</f>
         <v>45040</v>
@@ -2075,7 +2084,7 @@
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
-      <c r="T4" s="67"/>
+      <c r="T4" s="68"/>
       <c r="U4" s="9">
         <f>U5</f>
         <v>45047</v>
@@ -2085,7 +2094,7 @@
       <c r="X4" s="10"/>
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
-      <c r="AA4" s="67"/>
+      <c r="AA4" s="68"/>
       <c r="AB4" s="9">
         <f>AB5</f>
         <v>45054</v>
@@ -2095,7 +2104,7 @@
       <c r="AE4" s="10"/>
       <c r="AF4" s="10"/>
       <c r="AG4" s="10"/>
-      <c r="AH4" s="67"/>
+      <c r="AH4" s="68"/>
       <c r="AI4" s="9">
         <f>AI5</f>
         <v>45061</v>
@@ -2105,7 +2114,7 @@
       <c r="AL4" s="10"/>
       <c r="AM4" s="10"/>
       <c r="AN4" s="10"/>
-      <c r="AO4" s="67"/>
+      <c r="AO4" s="68"/>
       <c r="AP4" s="9">
         <f>AP5</f>
         <v>45068</v>
@@ -2115,7 +2124,7 @@
       <c r="AS4" s="10"/>
       <c r="AT4" s="10"/>
       <c r="AU4" s="10"/>
-      <c r="AV4" s="67"/>
+      <c r="AV4" s="68"/>
       <c r="AW4" s="9">
         <f>AW5</f>
         <v>45075</v>
@@ -2125,17 +2134,17 @@
       <c r="AZ4" s="10"/>
       <c r="BA4" s="10"/>
       <c r="BB4" s="10"/>
-      <c r="BC4" s="67"/>
-      <c r="BD4" s="74">
+      <c r="BC4" s="68"/>
+      <c r="BD4" s="75">
         <f>BD5</f>
         <v>45082</v>
       </c>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="80"/>
-      <c r="BG4" s="80"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="80"/>
-      <c r="BJ4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="81"/>
+      <c r="BI4" s="81"/>
+      <c r="BJ4" s="82"/>
     </row>
     <row r="5" spans="1:62">
       <c r="A5" s="11"/>
@@ -2168,7 +2177,7 @@
         <f t="shared" si="0"/>
         <v>45038</v>
       </c>
-      <c r="M5" s="68">
+      <c r="M5" s="69">
         <f t="shared" si="0"/>
         <v>45039</v>
       </c>
@@ -2196,7 +2205,7 @@
         <f t="shared" si="0"/>
         <v>45045</v>
       </c>
-      <c r="T5" s="68">
+      <c r="T5" s="69">
         <f t="shared" si="0"/>
         <v>45046</v>
       </c>
@@ -2224,7 +2233,7 @@
         <f t="shared" si="0"/>
         <v>45052</v>
       </c>
-      <c r="AA5" s="68">
+      <c r="AA5" s="69">
         <f t="shared" si="0"/>
         <v>45053</v>
       </c>
@@ -2252,7 +2261,7 @@
         <f t="shared" si="0"/>
         <v>45059</v>
       </c>
-      <c r="AH5" s="68">
+      <c r="AH5" s="69">
         <f t="shared" si="0"/>
         <v>45060</v>
       </c>
@@ -2280,7 +2289,7 @@
         <f t="shared" si="0"/>
         <v>45066</v>
       </c>
-      <c r="AO5" s="68">
+      <c r="AO5" s="69">
         <f t="shared" si="0"/>
         <v>45067</v>
       </c>
@@ -2308,7 +2317,7 @@
         <f t="shared" si="0"/>
         <v>45073</v>
       </c>
-      <c r="AV5" s="68">
+      <c r="AV5" s="69">
         <f t="shared" si="0"/>
         <v>45074</v>
       </c>
@@ -2336,35 +2345,35 @@
         <f t="shared" si="1"/>
         <v>45080</v>
       </c>
-      <c r="BC5" s="68">
+      <c r="BC5" s="69">
         <f t="shared" si="1"/>
         <v>45081</v>
       </c>
-      <c r="BD5" s="75">
+      <c r="BD5" s="76">
         <f t="shared" si="1"/>
         <v>45082</v>
       </c>
-      <c r="BE5" s="82">
+      <c r="BE5" s="83">
         <f t="shared" si="1"/>
         <v>45083</v>
       </c>
-      <c r="BF5" s="82">
+      <c r="BF5" s="83">
         <f t="shared" ref="BF5:BJ5" si="2">BE5+1</f>
         <v>45084</v>
       </c>
-      <c r="BG5" s="82">
+      <c r="BG5" s="83">
         <f t="shared" si="2"/>
         <v>45085</v>
       </c>
-      <c r="BH5" s="82">
+      <c r="BH5" s="83">
         <f t="shared" si="2"/>
         <v>45086</v>
       </c>
-      <c r="BI5" s="82">
+      <c r="BI5" s="83">
         <f t="shared" si="2"/>
         <v>45087</v>
       </c>
-      <c r="BJ5" s="83">
+      <c r="BJ5" s="84">
         <f t="shared" si="2"/>
         <v>45088</v>
       </c>
@@ -2580,31 +2589,31 @@
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="BD6" s="76" t="str">
+      <c r="BD6" s="77" t="str">
         <f t="shared" si="4"/>
         <v>M</v>
       </c>
-      <c r="BE6" s="76" t="str">
+      <c r="BE6" s="77" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="BF6" s="76" t="str">
+      <c r="BF6" s="77" t="str">
         <f t="shared" si="4"/>
         <v>W</v>
       </c>
-      <c r="BG6" s="76" t="str">
+      <c r="BG6" s="77" t="str">
         <f t="shared" si="4"/>
         <v>T</v>
       </c>
-      <c r="BH6" s="76" t="str">
+      <c r="BH6" s="77" t="str">
         <f t="shared" si="4"/>
         <v>F</v>
       </c>
-      <c r="BI6" s="76" t="str">
+      <c r="BI6" s="77" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
-      <c r="BJ6" s="76" t="str">
+      <c r="BJ6" s="77" t="str">
         <f t="shared" si="4"/>
         <v>S</v>
       </c>
@@ -2670,13 +2679,13 @@
       <c r="BA7" s="24"/>
       <c r="BB7" s="24"/>
       <c r="BC7" s="24"/>
-      <c r="BD7" s="77"/>
-      <c r="BE7" s="77"/>
-      <c r="BF7" s="77"/>
-      <c r="BG7" s="77"/>
-      <c r="BH7" s="77"/>
-      <c r="BI7" s="77"/>
-      <c r="BJ7" s="77"/>
+      <c r="BD7" s="78"/>
+      <c r="BE7" s="78"/>
+      <c r="BF7" s="78"/>
+      <c r="BG7" s="78"/>
+      <c r="BH7" s="78"/>
+      <c r="BI7" s="78"/>
+      <c r="BJ7" s="78"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A8" s="16"/>
@@ -2696,9 +2705,9 @@
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
       <c r="L8" s="24"/>
       <c r="M8" s="24"/>
       <c r="N8" s="24"/>
@@ -2743,13 +2752,13 @@
       <c r="BA8" s="24"/>
       <c r="BB8" s="24"/>
       <c r="BC8" s="24"/>
-      <c r="BD8" s="77"/>
-      <c r="BE8" s="77"/>
-      <c r="BF8" s="77"/>
-      <c r="BG8" s="77"/>
-      <c r="BH8" s="77"/>
-      <c r="BI8" s="77"/>
-      <c r="BJ8" s="77"/>
+      <c r="BD8" s="78"/>
+      <c r="BE8" s="78"/>
+      <c r="BF8" s="78"/>
+      <c r="BG8" s="78"/>
+      <c r="BH8" s="78"/>
+      <c r="BI8" s="78"/>
+      <c r="BJ8" s="78"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A9" s="16"/>
@@ -2769,9 +2778,9 @@
       </c>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
       <c r="L9" s="24"/>
       <c r="M9" s="24"/>
       <c r="N9" s="24"/>
@@ -2779,8 +2788,8 @@
       <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
-      <c r="S9" s="72"/>
-      <c r="T9" s="72"/>
+      <c r="S9" s="73"/>
+      <c r="T9" s="73"/>
       <c r="U9" s="24"/>
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
@@ -2816,13 +2825,13 @@
       <c r="BA9" s="24"/>
       <c r="BB9" s="24"/>
       <c r="BC9" s="24"/>
-      <c r="BD9" s="77"/>
-      <c r="BE9" s="77"/>
-      <c r="BF9" s="77"/>
-      <c r="BG9" s="77"/>
-      <c r="BH9" s="77"/>
-      <c r="BI9" s="77"/>
-      <c r="BJ9" s="77"/>
+      <c r="BD9" s="78"/>
+      <c r="BE9" s="78"/>
+      <c r="BF9" s="78"/>
+      <c r="BG9" s="78"/>
+      <c r="BH9" s="78"/>
+      <c r="BI9" s="78"/>
+      <c r="BJ9" s="78"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A10" s="16"/>
@@ -2842,9 +2851,9 @@
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="71"/>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
       <c r="N10" s="24"/>
@@ -2889,13 +2898,13 @@
       <c r="BA10" s="24"/>
       <c r="BB10" s="24"/>
       <c r="BC10" s="24"/>
-      <c r="BD10" s="77"/>
-      <c r="BE10" s="77"/>
-      <c r="BF10" s="77"/>
-      <c r="BG10" s="77"/>
-      <c r="BH10" s="77"/>
-      <c r="BI10" s="77"/>
-      <c r="BJ10" s="77"/>
+      <c r="BD10" s="78"/>
+      <c r="BE10" s="78"/>
+      <c r="BF10" s="78"/>
+      <c r="BG10" s="78"/>
+      <c r="BH10" s="78"/>
+      <c r="BI10" s="78"/>
+      <c r="BJ10" s="78"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A11" s="16"/>
@@ -2929,7 +2938,7 @@
       <c r="T11" s="24"/>
       <c r="U11" s="24"/>
       <c r="V11" s="24"/>
-      <c r="W11" s="72"/>
+      <c r="W11" s="73"/>
       <c r="X11" s="24"/>
       <c r="Y11" s="24"/>
       <c r="Z11" s="24"/>
@@ -2962,13 +2971,13 @@
       <c r="BA11" s="24"/>
       <c r="BB11" s="24"/>
       <c r="BC11" s="24"/>
-      <c r="BD11" s="77"/>
-      <c r="BE11" s="77"/>
-      <c r="BF11" s="77"/>
-      <c r="BG11" s="77"/>
-      <c r="BH11" s="77"/>
-      <c r="BI11" s="77"/>
-      <c r="BJ11" s="77"/>
+      <c r="BD11" s="78"/>
+      <c r="BE11" s="78"/>
+      <c r="BF11" s="78"/>
+      <c r="BG11" s="78"/>
+      <c r="BH11" s="78"/>
+      <c r="BI11" s="78"/>
+      <c r="BJ11" s="78"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A12" s="16"/>
@@ -3032,13 +3041,13 @@
       <c r="BA12" s="24"/>
       <c r="BB12" s="24"/>
       <c r="BC12" s="24"/>
-      <c r="BD12" s="77"/>
-      <c r="BE12" s="77"/>
-      <c r="BF12" s="77"/>
-      <c r="BG12" s="77"/>
-      <c r="BH12" s="77"/>
-      <c r="BI12" s="77"/>
-      <c r="BJ12" s="77"/>
+      <c r="BD12" s="78"/>
+      <c r="BE12" s="78"/>
+      <c r="BF12" s="78"/>
+      <c r="BG12" s="78"/>
+      <c r="BH12" s="78"/>
+      <c r="BI12" s="78"/>
+      <c r="BJ12" s="78"/>
     </row>
     <row r="13" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A13" s="16"/>
@@ -3102,13 +3111,13 @@
       <c r="BA13" s="24"/>
       <c r="BB13" s="24"/>
       <c r="BC13" s="24"/>
-      <c r="BD13" s="77"/>
-      <c r="BE13" s="77"/>
-      <c r="BF13" s="77"/>
-      <c r="BG13" s="77"/>
-      <c r="BH13" s="77"/>
-      <c r="BI13" s="77"/>
-      <c r="BJ13" s="77"/>
+      <c r="BD13" s="78"/>
+      <c r="BE13" s="78"/>
+      <c r="BF13" s="78"/>
+      <c r="BG13" s="78"/>
+      <c r="BH13" s="78"/>
+      <c r="BI13" s="78"/>
+      <c r="BJ13" s="78"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A14" s="16"/>
@@ -3130,23 +3139,23 @@
       <c r="O14" s="24"/>
       <c r="P14" s="24"/>
       <c r="Q14" s="24"/>
-      <c r="R14" s="71"/>
-      <c r="S14" s="71"/>
-      <c r="T14" s="71"/>
+      <c r="R14" s="72"/>
+      <c r="S14" s="72"/>
+      <c r="T14" s="72"/>
       <c r="U14" s="24"/>
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
-      <c r="Y14" s="73"/>
-      <c r="Z14" s="73"/>
-      <c r="AA14" s="73"/>
+      <c r="Y14" s="74"/>
+      <c r="Z14" s="74"/>
+      <c r="AA14" s="74"/>
       <c r="AB14" s="24"/>
       <c r="AC14" s="24"/>
       <c r="AD14" s="24"/>
       <c r="AE14" s="24"/>
-      <c r="AF14" s="73"/>
-      <c r="AG14" s="73"/>
-      <c r="AH14" s="73"/>
+      <c r="AF14" s="74"/>
+      <c r="AG14" s="74"/>
+      <c r="AH14" s="74"/>
       <c r="AI14" s="24"/>
       <c r="AJ14" s="24"/>
       <c r="AK14" s="24"/>
@@ -3163,18 +3172,18 @@
       <c r="AV14" s="24"/>
       <c r="AW14" s="24"/>
       <c r="AX14" s="24"/>
-      <c r="AY14" s="73"/>
-      <c r="AZ14" s="73"/>
-      <c r="BA14" s="73"/>
-      <c r="BB14" s="73"/>
-      <c r="BC14" s="73"/>
-      <c r="BD14" s="78"/>
-      <c r="BE14" s="78"/>
-      <c r="BF14" s="78"/>
-      <c r="BG14" s="78"/>
-      <c r="BH14" s="77"/>
-      <c r="BI14" s="77"/>
-      <c r="BJ14" s="77"/>
+      <c r="AY14" s="74"/>
+      <c r="AZ14" s="74"/>
+      <c r="BA14" s="74"/>
+      <c r="BB14" s="74"/>
+      <c r="BC14" s="74"/>
+      <c r="BD14" s="79"/>
+      <c r="BE14" s="79"/>
+      <c r="BF14" s="79"/>
+      <c r="BG14" s="79"/>
+      <c r="BH14" s="78"/>
+      <c r="BI14" s="78"/>
+      <c r="BJ14" s="78"/>
     </row>
     <row r="15" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A15" s="16"/>
@@ -3237,13 +3246,13 @@
       <c r="BA15" s="24"/>
       <c r="BB15" s="24"/>
       <c r="BC15" s="24"/>
-      <c r="BD15" s="77"/>
-      <c r="BE15" s="77"/>
-      <c r="BF15" s="77"/>
-      <c r="BG15" s="77"/>
-      <c r="BH15" s="77"/>
-      <c r="BI15" s="77"/>
-      <c r="BJ15" s="77"/>
+      <c r="BD15" s="78"/>
+      <c r="BE15" s="78"/>
+      <c r="BF15" s="78"/>
+      <c r="BG15" s="78"/>
+      <c r="BH15" s="78"/>
+      <c r="BI15" s="78"/>
+      <c r="BJ15" s="78"/>
     </row>
     <row r="16" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A16" s="16"/>
@@ -3310,13 +3319,13 @@
       <c r="BA16" s="24"/>
       <c r="BB16" s="24"/>
       <c r="BC16" s="24"/>
-      <c r="BD16" s="77"/>
-      <c r="BE16" s="77"/>
-      <c r="BF16" s="77"/>
-      <c r="BG16" s="77"/>
-      <c r="BH16" s="77"/>
-      <c r="BI16" s="77"/>
-      <c r="BJ16" s="77"/>
+      <c r="BD16" s="78"/>
+      <c r="BE16" s="78"/>
+      <c r="BF16" s="78"/>
+      <c r="BG16" s="78"/>
+      <c r="BH16" s="78"/>
+      <c r="BI16" s="78"/>
+      <c r="BJ16" s="78"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A17" s="16"/>
@@ -3346,8 +3355,8 @@
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
-      <c r="S17" s="72"/>
-      <c r="T17" s="72"/>
+      <c r="S17" s="73"/>
+      <c r="T17" s="73"/>
       <c r="U17" s="24"/>
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
@@ -3383,13 +3392,13 @@
       <c r="BA17" s="24"/>
       <c r="BB17" s="24"/>
       <c r="BC17" s="24"/>
-      <c r="BD17" s="77"/>
-      <c r="BE17" s="77"/>
-      <c r="BF17" s="77"/>
-      <c r="BG17" s="77"/>
-      <c r="BH17" s="77"/>
-      <c r="BI17" s="77"/>
-      <c r="BJ17" s="77"/>
+      <c r="BD17" s="78"/>
+      <c r="BE17" s="78"/>
+      <c r="BF17" s="78"/>
+      <c r="BG17" s="78"/>
+      <c r="BH17" s="78"/>
+      <c r="BI17" s="78"/>
+      <c r="BJ17" s="78"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A18" s="16"/>
@@ -3408,7 +3417,7 @@
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
       <c r="N18" s="24"/>
-      <c r="O18" s="71"/>
+      <c r="O18" s="72"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
@@ -3416,7 +3425,7 @@
       <c r="T18" s="24"/>
       <c r="U18" s="24"/>
       <c r="V18" s="24"/>
-      <c r="W18" s="72"/>
+      <c r="W18" s="73"/>
       <c r="X18" s="24"/>
       <c r="Y18" s="24"/>
       <c r="Z18" s="24"/>
@@ -3449,13 +3458,13 @@
       <c r="BA18" s="24"/>
       <c r="BB18" s="24"/>
       <c r="BC18" s="24"/>
-      <c r="BD18" s="77"/>
-      <c r="BE18" s="77"/>
-      <c r="BF18" s="77"/>
-      <c r="BG18" s="77"/>
-      <c r="BH18" s="77"/>
-      <c r="BI18" s="77"/>
-      <c r="BJ18" s="77"/>
+      <c r="BD18" s="78"/>
+      <c r="BE18" s="78"/>
+      <c r="BF18" s="78"/>
+      <c r="BG18" s="78"/>
+      <c r="BH18" s="78"/>
+      <c r="BI18" s="78"/>
+      <c r="BJ18" s="78"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A19" s="16"/>
@@ -3475,14 +3484,14 @@
       <c r="M19" s="24"/>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
-      <c r="P19" s="71"/>
-      <c r="Q19" s="71"/>
+      <c r="P19" s="72"/>
+      <c r="Q19" s="72"/>
       <c r="R19" s="24"/>
       <c r="S19" s="24"/>
       <c r="T19" s="24"/>
       <c r="U19" s="24"/>
       <c r="V19" s="24"/>
-      <c r="W19" s="72"/>
+      <c r="W19" s="73"/>
       <c r="X19" s="24"/>
       <c r="Y19" s="24"/>
       <c r="Z19" s="24"/>
@@ -3515,13 +3524,13 @@
       <c r="BA19" s="24"/>
       <c r="BB19" s="24"/>
       <c r="BC19" s="24"/>
-      <c r="BD19" s="77"/>
-      <c r="BE19" s="77"/>
-      <c r="BF19" s="77"/>
-      <c r="BG19" s="77"/>
-      <c r="BH19" s="77"/>
-      <c r="BI19" s="77"/>
-      <c r="BJ19" s="77"/>
+      <c r="BD19" s="78"/>
+      <c r="BE19" s="78"/>
+      <c r="BF19" s="78"/>
+      <c r="BG19" s="78"/>
+      <c r="BH19" s="78"/>
+      <c r="BI19" s="78"/>
+      <c r="BJ19" s="78"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A20" s="16"/>
@@ -3542,13 +3551,13 @@
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
       <c r="P20" s="24"/>
-      <c r="Q20" s="71"/>
-      <c r="R20" s="71"/>
+      <c r="Q20" s="72"/>
+      <c r="R20" s="72"/>
       <c r="S20" s="24"/>
       <c r="T20" s="24"/>
       <c r="U20" s="24"/>
       <c r="V20" s="24"/>
-      <c r="W20" s="72"/>
+      <c r="W20" s="73"/>
       <c r="X20" s="24"/>
       <c r="Y20" s="24"/>
       <c r="Z20" s="24"/>
@@ -3581,13 +3590,13 @@
       <c r="BA20" s="24"/>
       <c r="BB20" s="24"/>
       <c r="BC20" s="24"/>
-      <c r="BD20" s="77"/>
-      <c r="BE20" s="77"/>
-      <c r="BF20" s="77"/>
-      <c r="BG20" s="77"/>
-      <c r="BH20" s="77"/>
-      <c r="BI20" s="77"/>
-      <c r="BJ20" s="77"/>
+      <c r="BD20" s="78"/>
+      <c r="BE20" s="78"/>
+      <c r="BF20" s="78"/>
+      <c r="BG20" s="78"/>
+      <c r="BH20" s="78"/>
+      <c r="BI20" s="78"/>
+      <c r="BJ20" s="78"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A21" s="16"/>
@@ -3621,7 +3630,7 @@
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
-      <c r="W21" s="72"/>
+      <c r="W21" s="73"/>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
       <c r="Z21" s="24"/>
@@ -3654,13 +3663,13 @@
       <c r="BA21" s="24"/>
       <c r="BB21" s="24"/>
       <c r="BC21" s="24"/>
-      <c r="BD21" s="77"/>
-      <c r="BE21" s="77"/>
-      <c r="BF21" s="77"/>
-      <c r="BG21" s="77"/>
-      <c r="BH21" s="77"/>
-      <c r="BI21" s="77"/>
-      <c r="BJ21" s="77"/>
+      <c r="BD21" s="78"/>
+      <c r="BE21" s="78"/>
+      <c r="BF21" s="78"/>
+      <c r="BG21" s="78"/>
+      <c r="BH21" s="78"/>
+      <c r="BI21" s="78"/>
+      <c r="BJ21" s="78"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A22" s="16"/>
@@ -3686,12 +3695,12 @@
       <c r="O22" s="24"/>
       <c r="P22" s="24"/>
       <c r="Q22" s="24"/>
-      <c r="R22" s="70"/>
+      <c r="R22" s="71"/>
       <c r="S22" s="24"/>
       <c r="T22" s="24"/>
       <c r="U22" s="24"/>
       <c r="V22" s="24"/>
-      <c r="W22" s="72"/>
+      <c r="W22" s="73"/>
       <c r="X22" s="24"/>
       <c r="Y22" s="24"/>
       <c r="Z22" s="24"/>
@@ -3724,13 +3733,13 @@
       <c r="BA22" s="24"/>
       <c r="BB22" s="24"/>
       <c r="BC22" s="24"/>
-      <c r="BD22" s="77"/>
-      <c r="BE22" s="77"/>
-      <c r="BF22" s="77"/>
-      <c r="BG22" s="77"/>
-      <c r="BH22" s="77"/>
-      <c r="BI22" s="77"/>
-      <c r="BJ22" s="77"/>
+      <c r="BD22" s="78"/>
+      <c r="BE22" s="78"/>
+      <c r="BF22" s="78"/>
+      <c r="BG22" s="78"/>
+      <c r="BH22" s="78"/>
+      <c r="BI22" s="78"/>
+      <c r="BJ22" s="78"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A23" s="16"/>
@@ -3793,13 +3802,13 @@
       <c r="BA23" s="24"/>
       <c r="BB23" s="24"/>
       <c r="BC23" s="24"/>
-      <c r="BD23" s="77"/>
-      <c r="BE23" s="77"/>
-      <c r="BF23" s="77"/>
-      <c r="BG23" s="77"/>
-      <c r="BH23" s="77"/>
-      <c r="BI23" s="77"/>
-      <c r="BJ23" s="77"/>
+      <c r="BD23" s="78"/>
+      <c r="BE23" s="78"/>
+      <c r="BF23" s="78"/>
+      <c r="BG23" s="78"/>
+      <c r="BH23" s="78"/>
+      <c r="BI23" s="78"/>
+      <c r="BJ23" s="78"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A24" s="16"/>
@@ -3866,13 +3875,13 @@
       <c r="BA24" s="24"/>
       <c r="BB24" s="24"/>
       <c r="BC24" s="24"/>
-      <c r="BD24" s="77"/>
-      <c r="BE24" s="77"/>
-      <c r="BF24" s="77"/>
-      <c r="BG24" s="77"/>
-      <c r="BH24" s="77"/>
-      <c r="BI24" s="77"/>
-      <c r="BJ24" s="77"/>
+      <c r="BD24" s="78"/>
+      <c r="BE24" s="78"/>
+      <c r="BF24" s="78"/>
+      <c r="BG24" s="78"/>
+      <c r="BH24" s="78"/>
+      <c r="BI24" s="78"/>
+      <c r="BJ24" s="78"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A25" s="16"/>
@@ -3896,9 +3905,9 @@
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
       <c r="S25" s="24"/>
-      <c r="T25" s="71"/>
-      <c r="U25" s="71"/>
-      <c r="V25" s="71"/>
+      <c r="T25" s="72"/>
+      <c r="U25" s="72"/>
+      <c r="V25" s="72"/>
       <c r="W25" s="24"/>
       <c r="X25" s="24"/>
       <c r="Y25" s="24"/>
@@ -3932,13 +3941,13 @@
       <c r="BA25" s="24"/>
       <c r="BB25" s="24"/>
       <c r="BC25" s="24"/>
-      <c r="BD25" s="77"/>
-      <c r="BE25" s="77"/>
-      <c r="BF25" s="77"/>
-      <c r="BG25" s="77"/>
-      <c r="BH25" s="77"/>
-      <c r="BI25" s="77"/>
-      <c r="BJ25" s="77"/>
+      <c r="BD25" s="78"/>
+      <c r="BE25" s="78"/>
+      <c r="BF25" s="78"/>
+      <c r="BG25" s="78"/>
+      <c r="BH25" s="78"/>
+      <c r="BI25" s="78"/>
+      <c r="BJ25" s="78"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A26" s="16"/>
@@ -3965,8 +3974,8 @@
       <c r="T26" s="24"/>
       <c r="U26" s="24"/>
       <c r="V26" s="24"/>
-      <c r="W26" s="71"/>
-      <c r="X26" s="71"/>
+      <c r="W26" s="72"/>
+      <c r="X26" s="72"/>
       <c r="Y26" s="24"/>
       <c r="Z26" s="24"/>
       <c r="AA26" s="24"/>
@@ -3998,13 +4007,13 @@
       <c r="BA26" s="24"/>
       <c r="BB26" s="24"/>
       <c r="BC26" s="24"/>
-      <c r="BD26" s="77"/>
-      <c r="BE26" s="77"/>
-      <c r="BF26" s="77"/>
-      <c r="BG26" s="77"/>
-      <c r="BH26" s="77"/>
-      <c r="BI26" s="77"/>
-      <c r="BJ26" s="77"/>
+      <c r="BD26" s="78"/>
+      <c r="BE26" s="78"/>
+      <c r="BF26" s="78"/>
+      <c r="BG26" s="78"/>
+      <c r="BH26" s="78"/>
+      <c r="BI26" s="78"/>
+      <c r="BJ26" s="78"/>
     </row>
     <row r="27" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A27" s="16"/>
@@ -4071,17 +4080,17 @@
       <c r="BA27" s="24"/>
       <c r="BB27" s="24"/>
       <c r="BC27" s="24"/>
-      <c r="BD27" s="77"/>
-      <c r="BE27" s="77"/>
-      <c r="BF27" s="77"/>
-      <c r="BG27" s="77"/>
-      <c r="BH27" s="77"/>
-      <c r="BI27" s="77"/>
-      <c r="BJ27" s="77"/>
+      <c r="BD27" s="78"/>
+      <c r="BE27" s="78"/>
+      <c r="BF27" s="78"/>
+      <c r="BG27" s="78"/>
+      <c r="BH27" s="78"/>
+      <c r="BI27" s="78"/>
+      <c r="BJ27" s="78"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A28" s="16"/>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="41">
@@ -4144,13 +4153,13 @@
       <c r="BA28" s="24"/>
       <c r="BB28" s="24"/>
       <c r="BC28" s="24"/>
-      <c r="BD28" s="77"/>
-      <c r="BE28" s="77"/>
-      <c r="BF28" s="77"/>
-      <c r="BG28" s="77"/>
-      <c r="BH28" s="77"/>
-      <c r="BI28" s="77"/>
-      <c r="BJ28" s="77"/>
+      <c r="BD28" s="78"/>
+      <c r="BE28" s="78"/>
+      <c r="BF28" s="78"/>
+      <c r="BG28" s="78"/>
+      <c r="BH28" s="78"/>
+      <c r="BI28" s="78"/>
+      <c r="BJ28" s="78"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A29" s="16"/>
@@ -4213,13 +4222,13 @@
       <c r="BA29" s="24"/>
       <c r="BB29" s="24"/>
       <c r="BC29" s="24"/>
-      <c r="BD29" s="77"/>
-      <c r="BE29" s="77"/>
-      <c r="BF29" s="77"/>
-      <c r="BG29" s="77"/>
-      <c r="BH29" s="77"/>
-      <c r="BI29" s="77"/>
-      <c r="BJ29" s="77"/>
+      <c r="BD29" s="78"/>
+      <c r="BE29" s="78"/>
+      <c r="BF29" s="78"/>
+      <c r="BG29" s="78"/>
+      <c r="BH29" s="78"/>
+      <c r="BI29" s="78"/>
+      <c r="BJ29" s="78"/>
     </row>
     <row r="30" s="1" customFormat="1" ht="27" customHeight="1" spans="1:62">
       <c r="A30" s="16"/>
@@ -4286,13 +4295,13 @@
       <c r="BA30" s="24"/>
       <c r="BB30" s="24"/>
       <c r="BC30" s="24"/>
-      <c r="BD30" s="77"/>
-      <c r="BE30" s="77"/>
-      <c r="BF30" s="77"/>
-      <c r="BG30" s="77"/>
-      <c r="BH30" s="77"/>
-      <c r="BI30" s="77"/>
-      <c r="BJ30" s="77"/>
+      <c r="BD30" s="78"/>
+      <c r="BE30" s="78"/>
+      <c r="BF30" s="78"/>
+      <c r="BG30" s="78"/>
+      <c r="BH30" s="78"/>
+      <c r="BI30" s="78"/>
+      <c r="BJ30" s="78"/>
     </row>
     <row r="31" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A31" s="16"/>
@@ -4323,11 +4332,11 @@
       <c r="X31" s="24"/>
       <c r="Y31" s="24"/>
       <c r="Z31" s="24"/>
-      <c r="AA31" s="24"/>
-      <c r="AB31" s="24"/>
-      <c r="AC31" s="24"/>
-      <c r="AD31" s="24"/>
-      <c r="AE31" s="24"/>
+      <c r="AA31" s="72"/>
+      <c r="AB31" s="72"/>
+      <c r="AC31" s="72"/>
+      <c r="AD31" s="72"/>
+      <c r="AE31" s="72"/>
       <c r="AF31" s="24"/>
       <c r="AG31" s="24"/>
       <c r="AH31" s="24"/>
@@ -4352,17 +4361,17 @@
       <c r="BA31" s="24"/>
       <c r="BB31" s="24"/>
       <c r="BC31" s="24"/>
-      <c r="BD31" s="77"/>
-      <c r="BE31" s="77"/>
-      <c r="BF31" s="77"/>
-      <c r="BG31" s="77"/>
-      <c r="BH31" s="77"/>
-      <c r="BI31" s="77"/>
-      <c r="BJ31" s="77"/>
+      <c r="BD31" s="78"/>
+      <c r="BE31" s="78"/>
+      <c r="BF31" s="78"/>
+      <c r="BG31" s="78"/>
+      <c r="BH31" s="78"/>
+      <c r="BI31" s="78"/>
+      <c r="BJ31" s="78"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A32" s="16"/>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="49" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="47">
@@ -4425,17 +4434,17 @@
       <c r="BA32" s="24"/>
       <c r="BB32" s="24"/>
       <c r="BC32" s="24"/>
-      <c r="BD32" s="77"/>
-      <c r="BE32" s="77"/>
-      <c r="BF32" s="77"/>
-      <c r="BG32" s="77"/>
-      <c r="BH32" s="77"/>
-      <c r="BI32" s="77"/>
-      <c r="BJ32" s="77"/>
+      <c r="BD32" s="78"/>
+      <c r="BE32" s="78"/>
+      <c r="BF32" s="78"/>
+      <c r="BG32" s="78"/>
+      <c r="BH32" s="78"/>
+      <c r="BI32" s="78"/>
+      <c r="BJ32" s="78"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A33" s="16"/>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="49" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="47">
@@ -4498,21 +4507,21 @@
       <c r="BA33" s="24"/>
       <c r="BB33" s="24"/>
       <c r="BC33" s="24"/>
-      <c r="BD33" s="77"/>
-      <c r="BE33" s="77"/>
-      <c r="BF33" s="77"/>
-      <c r="BG33" s="77"/>
-      <c r="BH33" s="77"/>
-      <c r="BI33" s="77"/>
-      <c r="BJ33" s="77"/>
+      <c r="BD33" s="78"/>
+      <c r="BE33" s="78"/>
+      <c r="BF33" s="78"/>
+      <c r="BG33" s="78"/>
+      <c r="BH33" s="78"/>
+      <c r="BI33" s="78"/>
+      <c r="BJ33" s="78"/>
     </row>
-    <row r="34" s="1" customFormat="1" ht="21" spans="1:62">
+    <row r="34" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A34" s="16"/>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="52"/>
       <c r="E34" s="23"/>
       <c r="F34" s="23" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -4567,23 +4576,23 @@
       <c r="BA34" s="24"/>
       <c r="BB34" s="24"/>
       <c r="BC34" s="24"/>
-      <c r="BD34" s="77"/>
-      <c r="BE34" s="77"/>
-      <c r="BF34" s="77"/>
-      <c r="BG34" s="77"/>
-      <c r="BH34" s="77"/>
-      <c r="BI34" s="77"/>
-      <c r="BJ34" s="77"/>
+      <c r="BD34" s="78"/>
+      <c r="BE34" s="78"/>
+      <c r="BF34" s="78"/>
+      <c r="BG34" s="78"/>
+      <c r="BH34" s="78"/>
+      <c r="BI34" s="78"/>
+      <c r="BJ34" s="78"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A35" s="16"/>
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="53">
+      <c r="C35" s="54">
         <v>45060</v>
       </c>
-      <c r="D35" s="54">
+      <c r="D35" s="55">
         <v>45077</v>
       </c>
       <c r="E35" s="23"/>
@@ -4640,13 +4649,13 @@
       <c r="BA35" s="24"/>
       <c r="BB35" s="24"/>
       <c r="BC35" s="24"/>
-      <c r="BD35" s="77"/>
-      <c r="BE35" s="77"/>
-      <c r="BF35" s="77"/>
-      <c r="BG35" s="77"/>
-      <c r="BH35" s="77"/>
-      <c r="BI35" s="77"/>
-      <c r="BJ35" s="77"/>
+      <c r="BD35" s="78"/>
+      <c r="BE35" s="78"/>
+      <c r="BF35" s="78"/>
+      <c r="BG35" s="78"/>
+      <c r="BH35" s="78"/>
+      <c r="BI35" s="78"/>
+      <c r="BJ35" s="78"/>
     </row>
     <row r="36" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A36" s="16"/>
@@ -4684,16 +4693,16 @@
       <c r="AE36" s="24"/>
       <c r="AF36" s="24"/>
       <c r="AG36" s="24"/>
-      <c r="AH36" s="71"/>
-      <c r="AI36" s="71"/>
-      <c r="AJ36" s="71"/>
-      <c r="AK36" s="71"/>
-      <c r="AL36" s="71"/>
-      <c r="AM36" s="71"/>
-      <c r="AN36" s="71"/>
-      <c r="AO36" s="71"/>
-      <c r="AP36" s="71"/>
-      <c r="AQ36" s="71"/>
+      <c r="AH36" s="72"/>
+      <c r="AI36" s="72"/>
+      <c r="AJ36" s="72"/>
+      <c r="AK36" s="72"/>
+      <c r="AL36" s="72"/>
+      <c r="AM36" s="72"/>
+      <c r="AN36" s="72"/>
+      <c r="AO36" s="72"/>
+      <c r="AP36" s="72"/>
+      <c r="AQ36" s="72"/>
       <c r="AR36" s="24"/>
       <c r="AS36" s="24"/>
       <c r="AT36" s="24"/>
@@ -4706,13 +4715,13 @@
       <c r="BA36" s="24"/>
       <c r="BB36" s="24"/>
       <c r="BC36" s="24"/>
-      <c r="BD36" s="77"/>
-      <c r="BE36" s="77"/>
-      <c r="BF36" s="77"/>
-      <c r="BG36" s="77"/>
-      <c r="BH36" s="77"/>
-      <c r="BI36" s="77"/>
-      <c r="BJ36" s="77"/>
+      <c r="BD36" s="78"/>
+      <c r="BE36" s="78"/>
+      <c r="BF36" s="78"/>
+      <c r="BG36" s="78"/>
+      <c r="BH36" s="78"/>
+      <c r="BI36" s="78"/>
+      <c r="BJ36" s="78"/>
     </row>
     <row r="37" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A37" s="16"/>
@@ -4760,35 +4769,35 @@
       <c r="AO37" s="24"/>
       <c r="AP37" s="24"/>
       <c r="AQ37" s="24"/>
-      <c r="AR37" s="71"/>
-      <c r="AS37" s="71"/>
-      <c r="AT37" s="71"/>
-      <c r="AU37" s="71"/>
-      <c r="AV37" s="71"/>
-      <c r="AW37" s="71"/>
-      <c r="AX37" s="71"/>
-      <c r="AY37" s="71"/>
+      <c r="AR37" s="72"/>
+      <c r="AS37" s="72"/>
+      <c r="AT37" s="72"/>
+      <c r="AU37" s="72"/>
+      <c r="AV37" s="72"/>
+      <c r="AW37" s="72"/>
+      <c r="AX37" s="72"/>
+      <c r="AY37" s="72"/>
       <c r="AZ37" s="24"/>
       <c r="BA37" s="24"/>
       <c r="BB37" s="24"/>
       <c r="BC37" s="24"/>
-      <c r="BD37" s="77"/>
-      <c r="BE37" s="77"/>
-      <c r="BF37" s="77"/>
-      <c r="BG37" s="77"/>
-      <c r="BH37" s="77"/>
-      <c r="BI37" s="77"/>
-      <c r="BJ37" s="77"/>
+      <c r="BD37" s="78"/>
+      <c r="BE37" s="78"/>
+      <c r="BF37" s="78"/>
+      <c r="BG37" s="78"/>
+      <c r="BH37" s="78"/>
+      <c r="BI37" s="78"/>
+      <c r="BJ37" s="78"/>
     </row>
     <row r="38" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A38" s="16"/>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="53">
+      <c r="C38" s="54">
         <v>45072</v>
       </c>
-      <c r="D38" s="54">
+      <c r="D38" s="55">
         <v>45077</v>
       </c>
       <c r="E38" s="23"/>
@@ -4845,19 +4854,19 @@
       <c r="BA38" s="24"/>
       <c r="BB38" s="24"/>
       <c r="BC38" s="24"/>
-      <c r="BD38" s="77"/>
-      <c r="BE38" s="77"/>
-      <c r="BF38" s="77"/>
-      <c r="BG38" s="77"/>
-      <c r="BH38" s="77"/>
-      <c r="BI38" s="77"/>
-      <c r="BJ38" s="77"/>
+      <c r="BD38" s="78"/>
+      <c r="BE38" s="78"/>
+      <c r="BF38" s="78"/>
+      <c r="BG38" s="78"/>
+      <c r="BH38" s="78"/>
+      <c r="BI38" s="78"/>
+      <c r="BJ38" s="78"/>
     </row>
     <row r="39" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A39" s="16"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="57"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="58"/>
       <c r="E39" s="23"/>
       <c r="F39" s="23" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -4912,19 +4921,19 @@
       <c r="BA39" s="24"/>
       <c r="BB39" s="24"/>
       <c r="BC39" s="24"/>
-      <c r="BD39" s="77"/>
-      <c r="BE39" s="77"/>
-      <c r="BF39" s="77"/>
-      <c r="BG39" s="77"/>
-      <c r="BH39" s="77"/>
-      <c r="BI39" s="77"/>
-      <c r="BJ39" s="77"/>
+      <c r="BD39" s="78"/>
+      <c r="BE39" s="78"/>
+      <c r="BF39" s="78"/>
+      <c r="BG39" s="78"/>
+      <c r="BH39" s="78"/>
+      <c r="BI39" s="78"/>
+      <c r="BJ39" s="78"/>
     </row>
     <row r="40" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A40" s="16"/>
-      <c r="B40" s="55"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="57"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="58"/>
       <c r="E40" s="23"/>
       <c r="F40" s="23" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -4979,19 +4988,19 @@
       <c r="BA40" s="24"/>
       <c r="BB40" s="24"/>
       <c r="BC40" s="24"/>
-      <c r="BD40" s="77"/>
-      <c r="BE40" s="77"/>
-      <c r="BF40" s="77"/>
-      <c r="BG40" s="77"/>
-      <c r="BH40" s="77"/>
-      <c r="BI40" s="77"/>
-      <c r="BJ40" s="77"/>
+      <c r="BD40" s="78"/>
+      <c r="BE40" s="78"/>
+      <c r="BF40" s="78"/>
+      <c r="BG40" s="78"/>
+      <c r="BH40" s="78"/>
+      <c r="BI40" s="78"/>
+      <c r="BJ40" s="78"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A41" s="16"/>
-      <c r="B41" s="55"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="57"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="58"/>
       <c r="E41" s="23"/>
       <c r="F41" s="23" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -5046,82 +5055,82 @@
       <c r="BA41" s="24"/>
       <c r="BB41" s="24"/>
       <c r="BC41" s="24"/>
-      <c r="BD41" s="77"/>
-      <c r="BE41" s="77"/>
-      <c r="BF41" s="77"/>
-      <c r="BG41" s="77"/>
-      <c r="BH41" s="77"/>
-      <c r="BI41" s="77"/>
-      <c r="BJ41" s="77"/>
+      <c r="BD41" s="78"/>
+      <c r="BE41" s="78"/>
+      <c r="BF41" s="78"/>
+      <c r="BG41" s="78"/>
+      <c r="BH41" s="78"/>
+      <c r="BI41" s="78"/>
+      <c r="BJ41" s="78"/>
     </row>
     <row r="42" s="1" customFormat="1" ht="21.75" spans="1:62">
       <c r="A42" s="16"/>
-      <c r="B42" s="58" t="s">
+      <c r="B42" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="59"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61" t="str">
+      <c r="C42" s="60"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
-      <c r="K42" s="62"/>
-      <c r="L42" s="62"/>
-      <c r="M42" s="62"/>
-      <c r="N42" s="62"/>
-      <c r="O42" s="62"/>
-      <c r="P42" s="62"/>
-      <c r="Q42" s="62"/>
-      <c r="R42" s="62"/>
-      <c r="S42" s="62"/>
-      <c r="T42" s="62"/>
-      <c r="U42" s="62"/>
-      <c r="V42" s="62"/>
-      <c r="W42" s="62"/>
-      <c r="X42" s="62"/>
-      <c r="Y42" s="62"/>
-      <c r="Z42" s="62"/>
-      <c r="AA42" s="62"/>
-      <c r="AB42" s="62"/>
-      <c r="AC42" s="62"/>
-      <c r="AD42" s="62"/>
-      <c r="AE42" s="62"/>
-      <c r="AF42" s="62"/>
-      <c r="AG42" s="62"/>
-      <c r="AH42" s="62"/>
-      <c r="AI42" s="62"/>
-      <c r="AJ42" s="62"/>
-      <c r="AK42" s="62"/>
-      <c r="AL42" s="62"/>
-      <c r="AM42" s="62"/>
-      <c r="AN42" s="62"/>
-      <c r="AO42" s="62"/>
-      <c r="AP42" s="62"/>
-      <c r="AQ42" s="62"/>
-      <c r="AR42" s="62"/>
-      <c r="AS42" s="62"/>
-      <c r="AT42" s="62"/>
-      <c r="AU42" s="62"/>
-      <c r="AV42" s="62"/>
-      <c r="AW42" s="62"/>
-      <c r="AX42" s="62"/>
-      <c r="AY42" s="62"/>
-      <c r="AZ42" s="62"/>
-      <c r="BA42" s="62"/>
-      <c r="BB42" s="62"/>
-      <c r="BC42" s="62"/>
-      <c r="BD42" s="79"/>
-      <c r="BE42" s="79"/>
-      <c r="BF42" s="79"/>
-      <c r="BG42" s="79"/>
-      <c r="BH42" s="79"/>
-      <c r="BI42" s="79"/>
-      <c r="BJ42" s="79"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="63"/>
+      <c r="S42" s="63"/>
+      <c r="T42" s="63"/>
+      <c r="U42" s="63"/>
+      <c r="V42" s="63"/>
+      <c r="W42" s="63"/>
+      <c r="X42" s="63"/>
+      <c r="Y42" s="63"/>
+      <c r="Z42" s="63"/>
+      <c r="AA42" s="63"/>
+      <c r="AB42" s="63"/>
+      <c r="AC42" s="63"/>
+      <c r="AD42" s="63"/>
+      <c r="AE42" s="63"/>
+      <c r="AF42" s="63"/>
+      <c r="AG42" s="63"/>
+      <c r="AH42" s="63"/>
+      <c r="AI42" s="63"/>
+      <c r="AJ42" s="63"/>
+      <c r="AK42" s="63"/>
+      <c r="AL42" s="63"/>
+      <c r="AM42" s="63"/>
+      <c r="AN42" s="63"/>
+      <c r="AO42" s="63"/>
+      <c r="AP42" s="63"/>
+      <c r="AQ42" s="63"/>
+      <c r="AR42" s="63"/>
+      <c r="AS42" s="63"/>
+      <c r="AT42" s="63"/>
+      <c r="AU42" s="63"/>
+      <c r="AV42" s="63"/>
+      <c r="AW42" s="63"/>
+      <c r="AX42" s="63"/>
+      <c r="AY42" s="63"/>
+      <c r="AZ42" s="63"/>
+      <c r="BA42" s="63"/>
+      <c r="BB42" s="63"/>
+      <c r="BC42" s="63"/>
+      <c r="BD42" s="80"/>
+      <c r="BE42" s="80"/>
+      <c r="BF42" s="80"/>
+      <c r="BG42" s="80"/>
+      <c r="BH42" s="80"/>
+      <c r="BI42" s="80"/>
+      <c r="BJ42" s="80"/>
     </row>
     <row r="43" spans="1:55">
       <c r="A43" s="11"/>
@@ -5181,9 +5190,9 @@
       <c r="BC43" s="7"/>
     </row>
     <row r="44" spans="2:55">
-      <c r="B44" s="63"/>
+      <c r="B44" s="64"/>
       <c r="C44" s="12"/>
-      <c r="D44" s="64"/>
+      <c r="D44" s="65"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
@@ -5237,7 +5246,7 @@
       <c r="BC44" s="7"/>
     </row>
     <row r="45" spans="2:55">
-      <c r="B45" s="65"/>
+      <c r="B45" s="66"/>
       <c r="C45" s="12"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -5293,7 +5302,7 @@
       <c r="BC45" s="7"/>
     </row>
     <row r="46" spans="2:55">
-      <c r="B46" s="66"/>
+      <c r="B46" s="67"/>
       <c r="C46" s="12"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>

</xml_diff>